<commit_message>
Add test ltspice, schematics and other
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\university\Diploma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2D0F2A-AFE8-4049-8467-A55BCB59CFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3771A939-30BD-43F0-AD7A-4D678C828F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49E8A915-5A6F-4B3C-966A-272F8EBD50DB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Компоненты</t>
   </si>
@@ -52,13 +52,94 @@
   </si>
   <si>
     <t>Как подключить антенну:</t>
+  </si>
+  <si>
+    <t>В EasyEDA для SMD-конденсаторов использовать multulayer ceramic capacitor</t>
+  </si>
+  <si>
+    <t>f=700/(R*C)</t>
+  </si>
+  <si>
+    <t>R - сопротивление резисторов, которые стоят внутри, в кОм</t>
+  </si>
+  <si>
+    <t>С - в мкФ, способность конденсатора.</t>
+  </si>
+  <si>
+    <t>https://market-444.ru/article/details/glushilka-wifi-svoimi-rukami</t>
+  </si>
+  <si>
+    <t>https://podavitel.ru/glushilka-wi-fi-svoimi-rukami.html</t>
+  </si>
+  <si>
+    <t>Странные схемы глушилки</t>
+  </si>
+  <si>
+    <t>https://habr.com/ru/articles/356868/</t>
+  </si>
+  <si>
+    <t>Книги:</t>
+  </si>
+  <si>
+    <t>http://www.iqytechnicalcollege.com/EW%20102%20%20A%20Second%20Course%20in%20Electronic%20Warfare.pdf</t>
+  </si>
+  <si>
+    <t>https://core.ac.uk/download/pdf/232274856.pdf</t>
+  </si>
+  <si>
+    <t>Статьи:</t>
+  </si>
+  <si>
+    <t>Статья о влиянии шума на ofdm</t>
+  </si>
+  <si>
+    <t>https://overclockers.ru/blog/vovsir/show/50070/razbiraemsya-kak-rabotaet-wi-fi-pochemu-ne-nuzhen-moschnyj-router-i-chto-realno-vliyaet-na-rabotu-seti</t>
+  </si>
+  <si>
+    <t>шумы в wifi</t>
+  </si>
+  <si>
+    <t>Идеи:</t>
+  </si>
+  <si>
+    <t>Проверить, сколько битов передаётся в MSDA/PPDU wifi</t>
+  </si>
+  <si>
+    <t>Например передаётся 8 бит за 192us. Значит нам надо минимум 8 раз пройти по спектру wifi за 192us</t>
+  </si>
+  <si>
+    <t>идея для улучшения: для каждого спектра wifi использовать 1 ГУН. Так для всех спектров получится большое кол-во генераторов, однако производительность будет лучше.</t>
+  </si>
+  <si>
+    <t>https://libeldoc.bsuir.by/bitstream/123456789/37278/1/Muravev_2019.pdf</t>
+  </si>
+  <si>
+    <t>(поиск по слову "шум")</t>
+  </si>
+  <si>
+    <t>Уменьшаем ёмкость на C3 - получаем более короткие волны большего напряжения</t>
+  </si>
+  <si>
+    <t>Важно! При этом частота не меняется. Получаются короткие пики и большое равнины</t>
+  </si>
+  <si>
+    <t>Антенна (SMA-Male)</t>
+  </si>
+  <si>
+    <t>https://www.belchip.by/product/?selected_product=17702</t>
+  </si>
+  <si>
+    <t>Разъём (SMA-Female)</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/HjTech-HJSMA005/C1509228</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,14 +162,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -372,13 +465,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -399,30 +499,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -453,8 +529,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -475,16 +579,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>38607</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>181482</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>76201</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -514,8 +618,241 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4876801" y="2734182"/>
-          <a:ext cx="8610600" cy="3933317"/>
+          <a:off x="652744" y="2310600"/>
+          <a:ext cx="8547847" cy="3933317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>34883</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>29331</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>320511</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>29331</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2D0876A-237F-413B-BD4E-264DC3F1B8E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9716765" y="2348949"/>
+          <a:ext cx="7547040" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>132521</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>124238</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>24847</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>132521</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Oval 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6AF76DB-A829-487B-8C19-5A099AFEBCBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9939130" y="4530586"/>
+          <a:ext cx="1118152" cy="198783"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>268356</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>36442</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>91109</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>157369</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Oval 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F10F0E81-B414-4113-8957-3D8D49EEA839}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14978269" y="2728290"/>
+          <a:ext cx="1661492" cy="1073427"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>91965</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F89F1A4D-34DE-4630-AC5C-74B3E6F4F3F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="18211801" y="2419351"/>
+          <a:ext cx="7483364" cy="4324350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -834,178 +1171,349 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9202B416-C4F8-4CD1-A856-CE2988DE9FEF}">
-  <dimension ref="G1:U14"/>
+  <dimension ref="B1:AZ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:U8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="7:21" x14ac:dyDescent="0.25">
-      <c r="G1" s="2" t="s">
+    <row r="1" spans="2:52" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="4"/>
-    </row>
-    <row r="2" spans="7:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="7"/>
-    </row>
-    <row r="3" spans="7:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G3" s="22" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="6"/>
+    </row>
+    <row r="2" spans="2:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="9"/>
+    </row>
+    <row r="3" spans="2:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="25" t="s">
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="24"/>
-    </row>
-    <row r="4" spans="7:21" x14ac:dyDescent="0.25">
-      <c r="G4" s="16" t="s">
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="18"/>
+    </row>
+    <row r="4" spans="2:52" x14ac:dyDescent="0.25">
+      <c r="G4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="19" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="21"/>
-    </row>
-    <row r="5" spans="7:21" x14ac:dyDescent="0.25">
-      <c r="G5" s="9"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="10"/>
-    </row>
-    <row r="6" spans="7:21" x14ac:dyDescent="0.25">
-      <c r="G6" s="9"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="10"/>
-    </row>
-    <row r="7" spans="7:21" x14ac:dyDescent="0.25">
-      <c r="G7" s="9"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="10"/>
-    </row>
-    <row r="8" spans="7:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="13"/>
-    </row>
-    <row r="14" spans="7:21" x14ac:dyDescent="0.25">
-      <c r="I14" s="1" t="s">
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="15"/>
+      <c r="W4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:52" x14ac:dyDescent="0.25">
+      <c r="G5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="22"/>
+      <c r="W5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:52" x14ac:dyDescent="0.25">
+      <c r="G6" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="22"/>
+      <c r="W6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:52" x14ac:dyDescent="0.25">
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="22"/>
+      <c r="W7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+    </row>
+    <row r="8" spans="2:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="27"/>
+    </row>
+    <row r="11" spans="2:52" x14ac:dyDescent="0.25">
+      <c r="Y11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:52" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="Q12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="AA12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:52" x14ac:dyDescent="0.25">
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="2:52" x14ac:dyDescent="0.25">
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="AQ14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2"/>
+      <c r="AU14" s="2"/>
+      <c r="AV14" s="2"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2"/>
+      <c r="AZ14" s="2"/>
+    </row>
+    <row r="15" spans="2:52" x14ac:dyDescent="0.25">
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="AQ15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR15" s="2"/>
+      <c r="AS15" s="2"/>
+      <c r="AT15" s="2"/>
+      <c r="AU15" s="2"/>
+      <c r="AV15" s="2"/>
+      <c r="AW15" s="2"/>
+      <c r="AX15" s="2"/>
+      <c r="AY15" s="2"/>
+      <c r="AZ15" s="2"/>
+    </row>
+    <row r="16" spans="2:52" x14ac:dyDescent="0.25">
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="P40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" t="s">
+        <v>26</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="20">
+    <mergeCell ref="P41:T41"/>
+    <mergeCell ref="P42:T42"/>
+    <mergeCell ref="P43:T43"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="K8:U8"/>
-    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="K5:U5"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="K6:U6"/>
     <mergeCell ref="G7:J7"/>
     <mergeCell ref="K7:U7"/>
+    <mergeCell ref="AQ14:AZ14"/>
+    <mergeCell ref="AQ15:AZ15"/>
+    <mergeCell ref="W7:AA7"/>
     <mergeCell ref="G1:U2"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="K4:U4"/>
@@ -1014,9 +1522,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K4" r:id="rId1" xr:uid="{3340489E-6A80-4EDB-BA81-13E093DBD259}"/>
+    <hyperlink ref="K5" r:id="rId2" xr:uid="{8639ECCE-0F5D-4542-92B3-03A8EF4880F8}"/>
+    <hyperlink ref="K6" r:id="rId3" xr:uid="{52195850-7972-4858-AA25-A95B79761617}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add important chapter part
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\university\Diploma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A29EED8-7FBE-424D-A250-FCDDA6773640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70922965-E624-4FE3-9C50-1D28B135611F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49E8A915-5A6F-4B3C-966A-272F8EBD50DB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t>https://belchip.by/product/?selected_product=36951</t>
   </si>
@@ -319,6 +319,18 @@
   </si>
   <si>
     <t>https://jlcpcb.com/partdetail/Walsin_TechCorp-0201N1R5C250CT/C424820</t>
+  </si>
+  <si>
+    <t>Резистор 1к (х2)</t>
+  </si>
+  <si>
+    <t>Повышение частоты</t>
+  </si>
+  <si>
+    <t>WR20X1001FTL</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Walsin_TechCorp-WR20X1001FTL/C335021</t>
   </si>
 </sst>
 </file>
@@ -965,7 +977,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -980,6 +992,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -989,6 +1082,129 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="27" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="28" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -998,26 +1214,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1028,207 +1232,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="27" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="28" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1910,7 +1931,7 @@
   <dimension ref="B1:AZ78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH82" sqref="AH82"/>
+      <selection activeCell="W78" sqref="W78:Y78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,13 +2063,13 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
-      <c r="W7" s="22" t="s">
+      <c r="W7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="22"/>
-      <c r="Z7" s="22"/>
-      <c r="AA7" s="22"/>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="30"/>
     </row>
     <row r="8" spans="2:52" x14ac:dyDescent="0.25">
       <c r="G8" s="3"/>
@@ -2076,11 +2097,11 @@
       </c>
     </row>
     <row r="12" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
       <c r="Q12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2108,18 +2129,18 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
-      <c r="AQ14" s="18" t="s">
+      <c r="AQ14" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="AR14" s="18"/>
-      <c r="AS14" s="18"/>
-      <c r="AT14" s="18"/>
-      <c r="AU14" s="18"/>
-      <c r="AV14" s="18"/>
-      <c r="AW14" s="18"/>
-      <c r="AX14" s="18"/>
-      <c r="AY14" s="18"/>
-      <c r="AZ14" s="18"/>
+      <c r="AR14" s="22"/>
+      <c r="AS14" s="22"/>
+      <c r="AT14" s="22"/>
+      <c r="AU14" s="22"/>
+      <c r="AV14" s="22"/>
+      <c r="AW14" s="22"/>
+      <c r="AX14" s="22"/>
+      <c r="AY14" s="22"/>
+      <c r="AZ14" s="22"/>
     </row>
     <row r="15" spans="2:52" x14ac:dyDescent="0.25">
       <c r="Q15" s="1"/>
@@ -2128,18 +2149,18 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
-      <c r="AQ15" s="18" t="s">
+      <c r="AQ15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="AR15" s="18"/>
-      <c r="AS15" s="18"/>
-      <c r="AT15" s="18"/>
-      <c r="AU15" s="18"/>
-      <c r="AV15" s="18"/>
-      <c r="AW15" s="18"/>
-      <c r="AX15" s="18"/>
-      <c r="AY15" s="18"/>
-      <c r="AZ15" s="18"/>
+      <c r="AR15" s="22"/>
+      <c r="AS15" s="22"/>
+      <c r="AT15" s="22"/>
+      <c r="AU15" s="22"/>
+      <c r="AV15" s="22"/>
+      <c r="AW15" s="22"/>
+      <c r="AX15" s="22"/>
+      <c r="AY15" s="22"/>
+      <c r="AZ15" s="22"/>
     </row>
     <row r="16" spans="2:52" x14ac:dyDescent="0.25">
       <c r="Q16" s="1"/>
@@ -2161,13 +2182,13 @@
       <c r="B41" t="s">
         <v>14</v>
       </c>
-      <c r="P41" s="18" t="s">
+      <c r="P41" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="22"/>
+      <c r="S41" s="22"/>
+      <c r="T41" s="22"/>
       <c r="U41" t="s">
         <v>15</v>
       </c>
@@ -2179,23 +2200,23 @@
       <c r="J42" t="s">
         <v>25</v>
       </c>
-      <c r="P42" s="18" t="s">
+      <c r="P42" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="22"/>
       <c r="U42" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="18"/>
+      <c r="P43" s="22"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="22"/>
+      <c r="S43" s="22"/>
+      <c r="T43" s="22"/>
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
@@ -2217,980 +2238,960 @@
     </row>
     <row r="56" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="7"/>
-      <c r="P57" s="8"/>
-      <c r="R57" s="6" t="s">
+      <c r="C57" s="34"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="34"/>
+      <c r="K57" s="34"/>
+      <c r="L57" s="34"/>
+      <c r="M57" s="34"/>
+      <c r="N57" s="34"/>
+      <c r="O57" s="34"/>
+      <c r="P57" s="35"/>
+      <c r="R57" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="S57" s="7"/>
-      <c r="T57" s="7"/>
-      <c r="U57" s="7"/>
-      <c r="V57" s="7"/>
-      <c r="W57" s="7"/>
-      <c r="X57" s="7"/>
-      <c r="Y57" s="7"/>
-      <c r="Z57" s="7"/>
-      <c r="AA57" s="7"/>
-      <c r="AB57" s="7"/>
-      <c r="AC57" s="7"/>
-      <c r="AD57" s="7"/>
-      <c r="AE57" s="7"/>
-      <c r="AF57" s="7"/>
-      <c r="AG57" s="7"/>
-      <c r="AH57" s="7"/>
-      <c r="AI57" s="7"/>
-      <c r="AJ57" s="7"/>
-      <c r="AK57" s="7"/>
-      <c r="AL57" s="7"/>
-      <c r="AM57" s="7"/>
-      <c r="AN57" s="7"/>
-      <c r="AO57" s="7"/>
-      <c r="AP57" s="8"/>
+      <c r="S57" s="34"/>
+      <c r="T57" s="34"/>
+      <c r="U57" s="34"/>
+      <c r="V57" s="34"/>
+      <c r="W57" s="34"/>
+      <c r="X57" s="34"/>
+      <c r="Y57" s="34"/>
+      <c r="Z57" s="34"/>
+      <c r="AA57" s="34"/>
+      <c r="AB57" s="34"/>
+      <c r="AC57" s="34"/>
+      <c r="AD57" s="34"/>
+      <c r="AE57" s="34"/>
+      <c r="AF57" s="34"/>
+      <c r="AG57" s="34"/>
+      <c r="AH57" s="34"/>
+      <c r="AI57" s="34"/>
+      <c r="AJ57" s="34"/>
+      <c r="AK57" s="34"/>
+      <c r="AL57" s="34"/>
+      <c r="AM57" s="34"/>
+      <c r="AN57" s="34"/>
+      <c r="AO57" s="34"/>
+      <c r="AP57" s="35"/>
     </row>
     <row r="58" spans="2:42" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="31"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
-      <c r="I58" s="32"/>
-      <c r="J58" s="32"/>
-      <c r="K58" s="32"/>
-      <c r="L58" s="32"/>
-      <c r="M58" s="32"/>
-      <c r="N58" s="32"/>
-      <c r="O58" s="32"/>
-      <c r="P58" s="33"/>
-      <c r="R58" s="9"/>
-      <c r="S58" s="10"/>
-      <c r="T58" s="10"/>
-      <c r="U58" s="10"/>
-      <c r="V58" s="10"/>
-      <c r="W58" s="10"/>
-      <c r="X58" s="10"/>
-      <c r="Y58" s="10"/>
-      <c r="Z58" s="10"/>
-      <c r="AA58" s="10"/>
-      <c r="AB58" s="10"/>
-      <c r="AC58" s="10"/>
-      <c r="AD58" s="10"/>
-      <c r="AE58" s="10"/>
-      <c r="AF58" s="10"/>
-      <c r="AG58" s="10"/>
-      <c r="AH58" s="10"/>
-      <c r="AI58" s="10"/>
-      <c r="AJ58" s="10"/>
-      <c r="AK58" s="10"/>
-      <c r="AL58" s="10"/>
-      <c r="AM58" s="10"/>
-      <c r="AN58" s="10"/>
-      <c r="AO58" s="10"/>
-      <c r="AP58" s="11"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
+      <c r="L58" s="37"/>
+      <c r="M58" s="37"/>
+      <c r="N58" s="37"/>
+      <c r="O58" s="37"/>
+      <c r="P58" s="38"/>
+      <c r="R58" s="79"/>
+      <c r="S58" s="80"/>
+      <c r="T58" s="80"/>
+      <c r="U58" s="80"/>
+      <c r="V58" s="80"/>
+      <c r="W58" s="80"/>
+      <c r="X58" s="80"/>
+      <c r="Y58" s="80"/>
+      <c r="Z58" s="80"/>
+      <c r="AA58" s="80"/>
+      <c r="AB58" s="80"/>
+      <c r="AC58" s="80"/>
+      <c r="AD58" s="80"/>
+      <c r="AE58" s="80"/>
+      <c r="AF58" s="80"/>
+      <c r="AG58" s="80"/>
+      <c r="AH58" s="80"/>
+      <c r="AI58" s="80"/>
+      <c r="AJ58" s="80"/>
+      <c r="AK58" s="80"/>
+      <c r="AL58" s="80"/>
+      <c r="AM58" s="80"/>
+      <c r="AN58" s="80"/>
+      <c r="AO58" s="80"/>
+      <c r="AP58" s="81"/>
     </row>
     <row r="59" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="34" t="s">
+      <c r="B59" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C59" s="35"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="37" t="s">
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="G59" s="35"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="35"/>
-      <c r="M59" s="35"/>
-      <c r="N59" s="35"/>
-      <c r="O59" s="35"/>
-      <c r="P59" s="36"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="40"/>
+      <c r="J59" s="40"/>
+      <c r="K59" s="40"/>
+      <c r="L59" s="40"/>
+      <c r="M59" s="40"/>
+      <c r="N59" s="40"/>
+      <c r="O59" s="40"/>
+      <c r="P59" s="41"/>
       <c r="R59" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="S59" s="66" t="s">
+      <c r="S59" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="T59" s="67"/>
-      <c r="U59" s="67"/>
-      <c r="V59" s="68"/>
-      <c r="W59" s="19" t="s">
+      <c r="T59" s="51"/>
+      <c r="U59" s="51"/>
+      <c r="V59" s="52"/>
+      <c r="W59" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="X59" s="20"/>
-      <c r="Y59" s="21"/>
-      <c r="Z59" s="69" t="s">
+      <c r="X59" s="86"/>
+      <c r="Y59" s="87"/>
+      <c r="Z59" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="AA59" s="67"/>
-      <c r="AB59" s="67"/>
-      <c r="AC59" s="67"/>
-      <c r="AD59" s="67"/>
-      <c r="AE59" s="67"/>
-      <c r="AF59" s="67"/>
-      <c r="AG59" s="67"/>
-      <c r="AH59" s="67"/>
-      <c r="AI59" s="67"/>
-      <c r="AJ59" s="68"/>
-      <c r="AK59" s="66" t="s">
+      <c r="AA59" s="51"/>
+      <c r="AB59" s="51"/>
+      <c r="AC59" s="51"/>
+      <c r="AD59" s="51"/>
+      <c r="AE59" s="51"/>
+      <c r="AF59" s="51"/>
+      <c r="AG59" s="51"/>
+      <c r="AH59" s="51"/>
+      <c r="AI59" s="51"/>
+      <c r="AJ59" s="52"/>
+      <c r="AK59" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="AL59" s="67"/>
-      <c r="AM59" s="67"/>
-      <c r="AN59" s="67"/>
-      <c r="AO59" s="67"/>
-      <c r="AP59" s="70"/>
+      <c r="AL59" s="51"/>
+      <c r="AM59" s="51"/>
+      <c r="AN59" s="51"/>
+      <c r="AO59" s="51"/>
+      <c r="AP59" s="72"/>
     </row>
     <row r="60" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B60" s="25" t="s">
+      <c r="B60" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="38" t="s">
+      <c r="C60" s="44"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
-      <c r="L60" s="39"/>
-      <c r="M60" s="39"/>
-      <c r="N60" s="39"/>
-      <c r="O60" s="39"/>
-      <c r="P60" s="40"/>
-      <c r="R60" s="80">
+      <c r="G60" s="47"/>
+      <c r="H60" s="47"/>
+      <c r="I60" s="47"/>
+      <c r="J60" s="47"/>
+      <c r="K60" s="47"/>
+      <c r="L60" s="47"/>
+      <c r="M60" s="47"/>
+      <c r="N60" s="47"/>
+      <c r="O60" s="47"/>
+      <c r="P60" s="48"/>
+      <c r="R60" s="8">
         <v>1</v>
       </c>
-      <c r="S60" s="44" t="s">
+      <c r="S60" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="T60" s="45"/>
-      <c r="U60" s="45"/>
-      <c r="V60" s="46"/>
-      <c r="W60" s="84" t="s">
+      <c r="T60" s="55"/>
+      <c r="U60" s="55"/>
+      <c r="V60" s="56"/>
+      <c r="W60" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="X60" s="43"/>
-      <c r="Y60" s="81"/>
-      <c r="Z60" s="44" t="s">
+      <c r="X60" s="89"/>
+      <c r="Y60" s="90"/>
+      <c r="Z60" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="AA60" s="45"/>
-      <c r="AB60" s="45"/>
-      <c r="AC60" s="45"/>
-      <c r="AD60" s="45"/>
-      <c r="AE60" s="45"/>
-      <c r="AF60" s="45"/>
-      <c r="AG60" s="45"/>
-      <c r="AH60" s="45"/>
-      <c r="AI60" s="45"/>
-      <c r="AJ60" s="46"/>
-      <c r="AK60" s="87" t="s">
+      <c r="AA60" s="55"/>
+      <c r="AB60" s="55"/>
+      <c r="AC60" s="55"/>
+      <c r="AD60" s="55"/>
+      <c r="AE60" s="55"/>
+      <c r="AF60" s="55"/>
+      <c r="AG60" s="55"/>
+      <c r="AH60" s="55"/>
+      <c r="AI60" s="55"/>
+      <c r="AJ60" s="56"/>
+      <c r="AK60" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="AL60" s="71"/>
-      <c r="AM60" s="71"/>
-      <c r="AN60" s="71"/>
-      <c r="AO60" s="71"/>
-      <c r="AP60" s="72"/>
+      <c r="AL60" s="74"/>
+      <c r="AM60" s="74"/>
+      <c r="AN60" s="74"/>
+      <c r="AO60" s="74"/>
+      <c r="AP60" s="75"/>
     </row>
     <row r="61" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="29" t="s">
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
-      <c r="K61" s="13"/>
-      <c r="L61" s="13"/>
-      <c r="M61" s="13"/>
-      <c r="N61" s="13"/>
-      <c r="O61" s="13"/>
-      <c r="P61" s="14"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
+      <c r="M61" s="10"/>
+      <c r="N61" s="10"/>
+      <c r="O61" s="10"/>
+      <c r="P61" s="11"/>
       <c r="R61" s="4">
         <v>2</v>
       </c>
-      <c r="S61" s="41" t="s">
+      <c r="S61" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="T61" s="42"/>
-      <c r="U61" s="42"/>
-      <c r="V61" s="48"/>
-      <c r="W61" s="76" t="s">
+      <c r="T61" s="58"/>
+      <c r="U61" s="58"/>
+      <c r="V61" s="59"/>
+      <c r="W61" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="X61" s="47"/>
-      <c r="Y61" s="78"/>
-      <c r="Z61" s="41" t="s">
+      <c r="X61" s="27"/>
+      <c r="Y61" s="28"/>
+      <c r="Z61" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="AA61" s="42"/>
-      <c r="AB61" s="42"/>
-      <c r="AC61" s="42"/>
-      <c r="AD61" s="42"/>
-      <c r="AE61" s="42"/>
-      <c r="AF61" s="42"/>
-      <c r="AG61" s="42"/>
-      <c r="AH61" s="42"/>
-      <c r="AI61" s="42"/>
-      <c r="AJ61" s="48"/>
-      <c r="AK61" s="30" t="s">
+      <c r="AA61" s="58"/>
+      <c r="AB61" s="58"/>
+      <c r="AC61" s="58"/>
+      <c r="AD61" s="58"/>
+      <c r="AE61" s="58"/>
+      <c r="AF61" s="58"/>
+      <c r="AG61" s="58"/>
+      <c r="AH61" s="58"/>
+      <c r="AI61" s="58"/>
+      <c r="AJ61" s="59"/>
+      <c r="AK61" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AL61" s="13"/>
-      <c r="AM61" s="13"/>
-      <c r="AN61" s="13"/>
-      <c r="AO61" s="13"/>
-      <c r="AP61" s="14"/>
+      <c r="AL61" s="10"/>
+      <c r="AM61" s="10"/>
+      <c r="AN61" s="10"/>
+      <c r="AO61" s="10"/>
+      <c r="AP61" s="11"/>
     </row>
     <row r="62" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="29" t="s">
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
-      <c r="N62" s="13"/>
-      <c r="O62" s="13"/>
-      <c r="P62" s="14"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="10"/>
+      <c r="K62" s="10"/>
+      <c r="L62" s="10"/>
+      <c r="M62" s="10"/>
+      <c r="N62" s="10"/>
+      <c r="O62" s="10"/>
+      <c r="P62" s="11"/>
       <c r="R62" s="4">
         <v>3</v>
       </c>
-      <c r="S62" s="41" t="s">
+      <c r="S62" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="T62" s="42"/>
-      <c r="U62" s="42"/>
-      <c r="V62" s="48"/>
-      <c r="W62" s="76" t="s">
+      <c r="T62" s="58"/>
+      <c r="U62" s="58"/>
+      <c r="V62" s="59"/>
+      <c r="W62" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="X62" s="47"/>
-      <c r="Y62" s="78"/>
-      <c r="Z62" s="41" t="s">
+      <c r="X62" s="27"/>
+      <c r="Y62" s="28"/>
+      <c r="Z62" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="AA62" s="42"/>
-      <c r="AB62" s="42"/>
-      <c r="AC62" s="42"/>
-      <c r="AD62" s="42"/>
-      <c r="AE62" s="42"/>
-      <c r="AF62" s="42"/>
-      <c r="AG62" s="42"/>
-      <c r="AH62" s="42"/>
-      <c r="AI62" s="42"/>
-      <c r="AJ62" s="48"/>
-      <c r="AK62" s="30"/>
-      <c r="AL62" s="13"/>
-      <c r="AM62" s="13"/>
-      <c r="AN62" s="13"/>
-      <c r="AO62" s="13"/>
-      <c r="AP62" s="14"/>
+      <c r="AA62" s="58"/>
+      <c r="AB62" s="58"/>
+      <c r="AC62" s="58"/>
+      <c r="AD62" s="58"/>
+      <c r="AE62" s="58"/>
+      <c r="AF62" s="58"/>
+      <c r="AG62" s="58"/>
+      <c r="AH62" s="58"/>
+      <c r="AI62" s="58"/>
+      <c r="AJ62" s="59"/>
+      <c r="AK62" s="9"/>
+      <c r="AL62" s="10"/>
+      <c r="AM62" s="10"/>
+      <c r="AN62" s="10"/>
+      <c r="AO62" s="10"/>
+      <c r="AP62" s="11"/>
     </row>
     <row r="63" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B63" s="12"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
-      <c r="N63" s="13"/>
-      <c r="O63" s="13"/>
-      <c r="P63" s="14"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="10"/>
+      <c r="L63" s="10"/>
+      <c r="M63" s="10"/>
+      <c r="N63" s="10"/>
+      <c r="O63" s="10"/>
+      <c r="P63" s="11"/>
       <c r="R63" s="4">
         <v>4</v>
       </c>
-      <c r="S63" s="89" t="s">
+      <c r="S63" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="T63" s="73"/>
-      <c r="U63" s="73"/>
-      <c r="V63" s="90"/>
-      <c r="W63" s="76" t="s">
+      <c r="T63" s="61"/>
+      <c r="U63" s="61"/>
+      <c r="V63" s="62"/>
+      <c r="W63" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="X63" s="47"/>
-      <c r="Y63" s="78"/>
-      <c r="Z63" s="41" t="s">
+      <c r="X63" s="27"/>
+      <c r="Y63" s="28"/>
+      <c r="Z63" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="AA63" s="42"/>
-      <c r="AB63" s="42"/>
-      <c r="AC63" s="42"/>
-      <c r="AD63" s="42"/>
-      <c r="AE63" s="42"/>
-      <c r="AF63" s="42"/>
-      <c r="AG63" s="42"/>
-      <c r="AH63" s="42"/>
-      <c r="AI63" s="42"/>
-      <c r="AJ63" s="48"/>
-      <c r="AK63" s="30"/>
-      <c r="AL63" s="13"/>
-      <c r="AM63" s="13"/>
-      <c r="AN63" s="13"/>
-      <c r="AO63" s="13"/>
-      <c r="AP63" s="14"/>
+      <c r="AA63" s="58"/>
+      <c r="AB63" s="58"/>
+      <c r="AC63" s="58"/>
+      <c r="AD63" s="58"/>
+      <c r="AE63" s="58"/>
+      <c r="AF63" s="58"/>
+      <c r="AG63" s="58"/>
+      <c r="AH63" s="58"/>
+      <c r="AI63" s="58"/>
+      <c r="AJ63" s="59"/>
+      <c r="AK63" s="9"/>
+      <c r="AL63" s="10"/>
+      <c r="AM63" s="10"/>
+      <c r="AN63" s="10"/>
+      <c r="AO63" s="10"/>
+      <c r="AP63" s="11"/>
     </row>
     <row r="64" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="15"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="28"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
-      <c r="J64" s="16"/>
-      <c r="K64" s="16"/>
-      <c r="L64" s="16"/>
-      <c r="M64" s="16"/>
-      <c r="N64" s="16"/>
-      <c r="O64" s="16"/>
-      <c r="P64" s="17"/>
+      <c r="B64" s="49"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
+      <c r="J64" s="20"/>
+      <c r="K64" s="20"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="20"/>
+      <c r="N64" s="20"/>
+      <c r="O64" s="20"/>
+      <c r="P64" s="21"/>
       <c r="R64" s="4">
         <v>5</v>
       </c>
-      <c r="S64" s="49" t="s">
+      <c r="S64" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="T64" s="50"/>
-      <c r="U64" s="50"/>
-      <c r="V64" s="52"/>
-      <c r="W64" s="76" t="s">
+      <c r="T64" s="24"/>
+      <c r="U64" s="24"/>
+      <c r="V64" s="25"/>
+      <c r="W64" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="X64" s="47"/>
-      <c r="Y64" s="78"/>
-      <c r="Z64" s="51" t="s">
+      <c r="X64" s="27"/>
+      <c r="Y64" s="28"/>
+      <c r="Z64" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="AA64" s="50"/>
-      <c r="AB64" s="50"/>
-      <c r="AC64" s="50"/>
-      <c r="AD64" s="50"/>
-      <c r="AE64" s="50"/>
-      <c r="AF64" s="50"/>
-      <c r="AG64" s="50"/>
-      <c r="AH64" s="50"/>
-      <c r="AI64" s="50"/>
-      <c r="AJ64" s="52"/>
-      <c r="AK64" s="30"/>
-      <c r="AL64" s="13"/>
-      <c r="AM64" s="13"/>
-      <c r="AN64" s="13"/>
-      <c r="AO64" s="13"/>
-      <c r="AP64" s="14"/>
+      <c r="AA64" s="24"/>
+      <c r="AB64" s="24"/>
+      <c r="AC64" s="24"/>
+      <c r="AD64" s="24"/>
+      <c r="AE64" s="24"/>
+      <c r="AF64" s="24"/>
+      <c r="AG64" s="24"/>
+      <c r="AH64" s="24"/>
+      <c r="AI64" s="24"/>
+      <c r="AJ64" s="25"/>
+      <c r="AK64" s="9"/>
+      <c r="AL64" s="10"/>
+      <c r="AM64" s="10"/>
+      <c r="AN64" s="10"/>
+      <c r="AO64" s="10"/>
+      <c r="AP64" s="11"/>
     </row>
     <row r="65" spans="2:42" x14ac:dyDescent="0.25">
       <c r="R65" s="4">
         <v>6</v>
       </c>
-      <c r="S65" s="49" t="s">
+      <c r="S65" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="T65" s="50"/>
-      <c r="U65" s="50"/>
-      <c r="V65" s="52"/>
-      <c r="W65" s="76" t="s">
+      <c r="T65" s="24"/>
+      <c r="U65" s="24"/>
+      <c r="V65" s="25"/>
+      <c r="W65" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="X65" s="47"/>
-      <c r="Y65" s="78"/>
-      <c r="Z65" s="51" t="s">
+      <c r="X65" s="27"/>
+      <c r="Y65" s="28"/>
+      <c r="Z65" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="AA65" s="50"/>
-      <c r="AB65" s="50"/>
-      <c r="AC65" s="50"/>
-      <c r="AD65" s="50"/>
-      <c r="AE65" s="50"/>
-      <c r="AF65" s="50"/>
-      <c r="AG65" s="50"/>
-      <c r="AH65" s="50"/>
-      <c r="AI65" s="50"/>
-      <c r="AJ65" s="52"/>
-      <c r="AK65" s="30"/>
-      <c r="AL65" s="13"/>
-      <c r="AM65" s="13"/>
-      <c r="AN65" s="13"/>
-      <c r="AO65" s="13"/>
-      <c r="AP65" s="14"/>
+      <c r="AA65" s="24"/>
+      <c r="AB65" s="24"/>
+      <c r="AC65" s="24"/>
+      <c r="AD65" s="24"/>
+      <c r="AE65" s="24"/>
+      <c r="AF65" s="24"/>
+      <c r="AG65" s="24"/>
+      <c r="AH65" s="24"/>
+      <c r="AI65" s="24"/>
+      <c r="AJ65" s="25"/>
+      <c r="AK65" s="9"/>
+      <c r="AL65" s="10"/>
+      <c r="AM65" s="10"/>
+      <c r="AN65" s="10"/>
+      <c r="AO65" s="10"/>
+      <c r="AP65" s="11"/>
     </row>
     <row r="66" spans="2:42" x14ac:dyDescent="0.25">
       <c r="R66" s="4">
         <v>7</v>
       </c>
-      <c r="S66" s="49" t="s">
+      <c r="S66" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="T66" s="50"/>
-      <c r="U66" s="50"/>
-      <c r="V66" s="52"/>
-      <c r="W66" s="76" t="s">
+      <c r="T66" s="92"/>
+      <c r="U66" s="92"/>
+      <c r="V66" s="93"/>
+      <c r="W66" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="X66" s="47"/>
-      <c r="Y66" s="78"/>
-      <c r="Z66" s="51" t="s">
+      <c r="X66" s="27"/>
+      <c r="Y66" s="28"/>
+      <c r="Z66" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="AA66" s="50"/>
-      <c r="AB66" s="50"/>
-      <c r="AC66" s="50"/>
-      <c r="AD66" s="50"/>
-      <c r="AE66" s="50"/>
-      <c r="AF66" s="50"/>
-      <c r="AG66" s="50"/>
-      <c r="AH66" s="50"/>
-      <c r="AI66" s="50"/>
-      <c r="AJ66" s="52"/>
-      <c r="AK66" s="30"/>
-      <c r="AL66" s="13"/>
-      <c r="AM66" s="13"/>
-      <c r="AN66" s="13"/>
-      <c r="AO66" s="13"/>
-      <c r="AP66" s="14"/>
+      <c r="AA66" s="24"/>
+      <c r="AB66" s="24"/>
+      <c r="AC66" s="24"/>
+      <c r="AD66" s="24"/>
+      <c r="AE66" s="24"/>
+      <c r="AF66" s="24"/>
+      <c r="AG66" s="24"/>
+      <c r="AH66" s="24"/>
+      <c r="AI66" s="24"/>
+      <c r="AJ66" s="25"/>
+      <c r="AK66" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL66" s="10"/>
+      <c r="AM66" s="10"/>
+      <c r="AN66" s="10"/>
+      <c r="AO66" s="10"/>
+      <c r="AP66" s="11"/>
     </row>
     <row r="67" spans="2:42" x14ac:dyDescent="0.25">
       <c r="R67" s="4">
         <v>8</v>
       </c>
-      <c r="S67" s="49" t="s">
+      <c r="S67" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="T67" s="50"/>
-      <c r="U67" s="50"/>
-      <c r="V67" s="52"/>
-      <c r="W67" s="76" t="s">
+      <c r="T67" s="24"/>
+      <c r="U67" s="24"/>
+      <c r="V67" s="25"/>
+      <c r="W67" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="X67" s="47"/>
-      <c r="Y67" s="78"/>
-      <c r="Z67" s="51" t="s">
+      <c r="X67" s="27"/>
+      <c r="Y67" s="28"/>
+      <c r="Z67" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="AA67" s="50"/>
-      <c r="AB67" s="50"/>
-      <c r="AC67" s="50"/>
-      <c r="AD67" s="50"/>
-      <c r="AE67" s="50"/>
-      <c r="AF67" s="50"/>
-      <c r="AG67" s="50"/>
-      <c r="AH67" s="50"/>
-      <c r="AI67" s="50"/>
-      <c r="AJ67" s="52"/>
-      <c r="AK67" s="30"/>
-      <c r="AL67" s="13"/>
-      <c r="AM67" s="13"/>
-      <c r="AN67" s="13"/>
-      <c r="AO67" s="13"/>
-      <c r="AP67" s="14"/>
+      <c r="AA67" s="24"/>
+      <c r="AB67" s="24"/>
+      <c r="AC67" s="24"/>
+      <c r="AD67" s="24"/>
+      <c r="AE67" s="24"/>
+      <c r="AF67" s="24"/>
+      <c r="AG67" s="24"/>
+      <c r="AH67" s="24"/>
+      <c r="AI67" s="24"/>
+      <c r="AJ67" s="25"/>
+      <c r="AK67" s="9"/>
+      <c r="AL67" s="10"/>
+      <c r="AM67" s="10"/>
+      <c r="AN67" s="10"/>
+      <c r="AO67" s="10"/>
+      <c r="AP67" s="11"/>
     </row>
     <row r="68" spans="2:42" x14ac:dyDescent="0.25">
       <c r="R68" s="4">
         <v>9</v>
       </c>
-      <c r="S68" s="49" t="s">
+      <c r="S68" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="T68" s="50"/>
-      <c r="U68" s="50"/>
-      <c r="V68" s="52"/>
-      <c r="W68" s="76" t="s">
+      <c r="T68" s="24"/>
+      <c r="U68" s="24"/>
+      <c r="V68" s="25"/>
+      <c r="W68" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="X68" s="47"/>
-      <c r="Y68" s="78"/>
-      <c r="Z68" s="51" t="s">
+      <c r="X68" s="27"/>
+      <c r="Y68" s="28"/>
+      <c r="Z68" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="AA68" s="50"/>
-      <c r="AB68" s="50"/>
-      <c r="AC68" s="50"/>
-      <c r="AD68" s="50"/>
-      <c r="AE68" s="50"/>
-      <c r="AF68" s="50"/>
-      <c r="AG68" s="50"/>
-      <c r="AH68" s="50"/>
-      <c r="AI68" s="50"/>
-      <c r="AJ68" s="52"/>
-      <c r="AK68" s="30"/>
-      <c r="AL68" s="13"/>
-      <c r="AM68" s="13"/>
-      <c r="AN68" s="13"/>
-      <c r="AO68" s="13"/>
-      <c r="AP68" s="14"/>
+      <c r="AA68" s="24"/>
+      <c r="AB68" s="24"/>
+      <c r="AC68" s="24"/>
+      <c r="AD68" s="24"/>
+      <c r="AE68" s="24"/>
+      <c r="AF68" s="24"/>
+      <c r="AG68" s="24"/>
+      <c r="AH68" s="24"/>
+      <c r="AI68" s="24"/>
+      <c r="AJ68" s="25"/>
+      <c r="AK68" s="9"/>
+      <c r="AL68" s="10"/>
+      <c r="AM68" s="10"/>
+      <c r="AN68" s="10"/>
+      <c r="AO68" s="10"/>
+      <c r="AP68" s="11"/>
     </row>
     <row r="69" spans="2:42" x14ac:dyDescent="0.25">
       <c r="R69" s="4">
         <v>10</v>
       </c>
-      <c r="S69" s="49" t="s">
+      <c r="S69" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="T69" s="50"/>
-      <c r="U69" s="50"/>
-      <c r="V69" s="52"/>
-      <c r="W69" s="76" t="s">
+      <c r="T69" s="24"/>
+      <c r="U69" s="24"/>
+      <c r="V69" s="25"/>
+      <c r="W69" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="X69" s="47"/>
-      <c r="Y69" s="78"/>
-      <c r="Z69" s="51" t="s">
+      <c r="X69" s="27"/>
+      <c r="Y69" s="28"/>
+      <c r="Z69" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="AA69" s="50"/>
-      <c r="AB69" s="50"/>
-      <c r="AC69" s="50"/>
-      <c r="AD69" s="50"/>
-      <c r="AE69" s="50"/>
-      <c r="AF69" s="50"/>
-      <c r="AG69" s="50"/>
-      <c r="AH69" s="50"/>
-      <c r="AI69" s="50"/>
-      <c r="AJ69" s="52"/>
-      <c r="AK69" s="30"/>
-      <c r="AL69" s="13"/>
-      <c r="AM69" s="13"/>
-      <c r="AN69" s="13"/>
-      <c r="AO69" s="13"/>
-      <c r="AP69" s="14"/>
+      <c r="AA69" s="24"/>
+      <c r="AB69" s="24"/>
+      <c r="AC69" s="24"/>
+      <c r="AD69" s="24"/>
+      <c r="AE69" s="24"/>
+      <c r="AF69" s="24"/>
+      <c r="AG69" s="24"/>
+      <c r="AH69" s="24"/>
+      <c r="AI69" s="24"/>
+      <c r="AJ69" s="25"/>
+      <c r="AK69" s="9"/>
+      <c r="AL69" s="10"/>
+      <c r="AM69" s="10"/>
+      <c r="AN69" s="10"/>
+      <c r="AO69" s="10"/>
+      <c r="AP69" s="11"/>
     </row>
     <row r="70" spans="2:42" x14ac:dyDescent="0.25">
       <c r="R70" s="4">
         <v>11</v>
       </c>
-      <c r="S70" s="49" t="s">
+      <c r="S70" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="T70" s="50"/>
-      <c r="U70" s="50"/>
-      <c r="V70" s="52"/>
-      <c r="W70" s="76" t="s">
+      <c r="T70" s="24"/>
+      <c r="U70" s="24"/>
+      <c r="V70" s="25"/>
+      <c r="W70" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="X70" s="47"/>
-      <c r="Y70" s="78"/>
-      <c r="Z70" s="51" t="s">
+      <c r="X70" s="27"/>
+      <c r="Y70" s="28"/>
+      <c r="Z70" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="AA70" s="50"/>
-      <c r="AB70" s="50"/>
-      <c r="AC70" s="50"/>
-      <c r="AD70" s="50"/>
-      <c r="AE70" s="50"/>
-      <c r="AF70" s="50"/>
-      <c r="AG70" s="50"/>
-      <c r="AH70" s="50"/>
-      <c r="AI70" s="50"/>
-      <c r="AJ70" s="52"/>
-      <c r="AK70" s="30"/>
-      <c r="AL70" s="13"/>
-      <c r="AM70" s="13"/>
-      <c r="AN70" s="13"/>
-      <c r="AO70" s="13"/>
-      <c r="AP70" s="14"/>
+      <c r="AA70" s="24"/>
+      <c r="AB70" s="24"/>
+      <c r="AC70" s="24"/>
+      <c r="AD70" s="24"/>
+      <c r="AE70" s="24"/>
+      <c r="AF70" s="24"/>
+      <c r="AG70" s="24"/>
+      <c r="AH70" s="24"/>
+      <c r="AI70" s="24"/>
+      <c r="AJ70" s="25"/>
+      <c r="AK70" s="9"/>
+      <c r="AL70" s="10"/>
+      <c r="AM70" s="10"/>
+      <c r="AN70" s="10"/>
+      <c r="AO70" s="10"/>
+      <c r="AP70" s="11"/>
     </row>
     <row r="71" spans="2:42" x14ac:dyDescent="0.25">
       <c r="R71" s="4">
         <v>12</v>
       </c>
-      <c r="S71" s="49" t="s">
+      <c r="S71" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="T71" s="50"/>
-      <c r="U71" s="50"/>
-      <c r="V71" s="52"/>
-      <c r="W71" s="76" t="s">
+      <c r="T71" s="24"/>
+      <c r="U71" s="24"/>
+      <c r="V71" s="25"/>
+      <c r="W71" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="X71" s="47"/>
-      <c r="Y71" s="78"/>
-      <c r="Z71" s="51" t="s">
+      <c r="X71" s="27"/>
+      <c r="Y71" s="28"/>
+      <c r="Z71" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="AA71" s="50"/>
-      <c r="AB71" s="50"/>
-      <c r="AC71" s="50"/>
-      <c r="AD71" s="50"/>
-      <c r="AE71" s="50"/>
-      <c r="AF71" s="50"/>
-      <c r="AG71" s="50"/>
-      <c r="AH71" s="50"/>
-      <c r="AI71" s="50"/>
-      <c r="AJ71" s="52"/>
-      <c r="AK71" s="30"/>
-      <c r="AL71" s="13"/>
-      <c r="AM71" s="13"/>
-      <c r="AN71" s="13"/>
-      <c r="AO71" s="13"/>
-      <c r="AP71" s="14"/>
+      <c r="AA71" s="24"/>
+      <c r="AB71" s="24"/>
+      <c r="AC71" s="24"/>
+      <c r="AD71" s="24"/>
+      <c r="AE71" s="24"/>
+      <c r="AF71" s="24"/>
+      <c r="AG71" s="24"/>
+      <c r="AH71" s="24"/>
+      <c r="AI71" s="24"/>
+      <c r="AJ71" s="25"/>
+      <c r="AK71" s="9"/>
+      <c r="AL71" s="10"/>
+      <c r="AM71" s="10"/>
+      <c r="AN71" s="10"/>
+      <c r="AO71" s="10"/>
+      <c r="AP71" s="11"/>
     </row>
     <row r="72" spans="2:42" x14ac:dyDescent="0.25">
       <c r="R72" s="4">
         <v>13</v>
       </c>
-      <c r="S72" s="49" t="s">
+      <c r="S72" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="T72" s="50"/>
-      <c r="U72" s="50"/>
-      <c r="V72" s="52"/>
-      <c r="W72" s="85" t="s">
+      <c r="T72" s="24"/>
+      <c r="U72" s="24"/>
+      <c r="V72" s="25"/>
+      <c r="W72" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="X72" s="57"/>
-      <c r="Y72" s="82"/>
-      <c r="Z72" s="51" t="s">
+      <c r="X72" s="77"/>
+      <c r="Y72" s="78"/>
+      <c r="Z72" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="AA72" s="50"/>
-      <c r="AB72" s="50"/>
-      <c r="AC72" s="50"/>
-      <c r="AD72" s="50"/>
-      <c r="AE72" s="50"/>
-      <c r="AF72" s="50"/>
-      <c r="AG72" s="50"/>
-      <c r="AH72" s="50"/>
-      <c r="AI72" s="50"/>
-      <c r="AJ72" s="52"/>
-      <c r="AK72" s="30"/>
-      <c r="AL72" s="13"/>
-      <c r="AM72" s="13"/>
-      <c r="AN72" s="13"/>
-      <c r="AO72" s="13"/>
-      <c r="AP72" s="14"/>
+      <c r="AA72" s="24"/>
+      <c r="AB72" s="24"/>
+      <c r="AC72" s="24"/>
+      <c r="AD72" s="24"/>
+      <c r="AE72" s="24"/>
+      <c r="AF72" s="24"/>
+      <c r="AG72" s="24"/>
+      <c r="AH72" s="24"/>
+      <c r="AI72" s="24"/>
+      <c r="AJ72" s="25"/>
+      <c r="AK72" s="9"/>
+      <c r="AL72" s="10"/>
+      <c r="AM72" s="10"/>
+      <c r="AN72" s="10"/>
+      <c r="AO72" s="10"/>
+      <c r="AP72" s="11"/>
     </row>
     <row r="73" spans="2:42" x14ac:dyDescent="0.25">
       <c r="R73" s="4">
         <v>14</v>
       </c>
-      <c r="S73" s="49" t="s">
+      <c r="S73" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="T73" s="50"/>
-      <c r="U73" s="50"/>
-      <c r="V73" s="52"/>
-      <c r="W73" s="76" t="s">
+      <c r="T73" s="24"/>
+      <c r="U73" s="24"/>
+      <c r="V73" s="25"/>
+      <c r="W73" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="X73" s="47"/>
-      <c r="Y73" s="78"/>
-      <c r="Z73" s="51" t="s">
+      <c r="X73" s="27"/>
+      <c r="Y73" s="28"/>
+      <c r="Z73" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="AA73" s="50"/>
-      <c r="AB73" s="50"/>
-      <c r="AC73" s="50"/>
-      <c r="AD73" s="50"/>
-      <c r="AE73" s="50"/>
-      <c r="AF73" s="50"/>
-      <c r="AG73" s="50"/>
-      <c r="AH73" s="50"/>
-      <c r="AI73" s="50"/>
-      <c r="AJ73" s="52"/>
-      <c r="AK73" s="30"/>
-      <c r="AL73" s="13"/>
-      <c r="AM73" s="13"/>
-      <c r="AN73" s="13"/>
-      <c r="AO73" s="13"/>
-      <c r="AP73" s="14"/>
+      <c r="AA73" s="24"/>
+      <c r="AB73" s="24"/>
+      <c r="AC73" s="24"/>
+      <c r="AD73" s="24"/>
+      <c r="AE73" s="24"/>
+      <c r="AF73" s="24"/>
+      <c r="AG73" s="24"/>
+      <c r="AH73" s="24"/>
+      <c r="AI73" s="24"/>
+      <c r="AJ73" s="25"/>
+      <c r="AK73" s="9"/>
+      <c r="AL73" s="10"/>
+      <c r="AM73" s="10"/>
+      <c r="AN73" s="10"/>
+      <c r="AO73" s="10"/>
+      <c r="AP73" s="11"/>
     </row>
     <row r="74" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B74" s="22" t="s">
+      <c r="B74" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
-      <c r="F74" s="18" t="s">
+      <c r="C74" s="30"/>
+      <c r="D74" s="30"/>
+      <c r="F74" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="18"/>
-      <c r="L74" s="18"/>
-      <c r="M74" s="18"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="22"/>
+      <c r="K74" s="22"/>
+      <c r="L74" s="22"/>
+      <c r="M74" s="22"/>
       <c r="R74" s="4">
         <v>15</v>
       </c>
-      <c r="S74" s="49" t="s">
+      <c r="S74" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="T74" s="50"/>
-      <c r="U74" s="50"/>
-      <c r="V74" s="52"/>
-      <c r="W74" s="76" t="s">
+      <c r="T74" s="24"/>
+      <c r="U74" s="24"/>
+      <c r="V74" s="25"/>
+      <c r="W74" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="X74" s="47"/>
-      <c r="Y74" s="78"/>
-      <c r="Z74" s="51" t="s">
+      <c r="X74" s="27"/>
+      <c r="Y74" s="28"/>
+      <c r="Z74" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="AA74" s="50"/>
-      <c r="AB74" s="50"/>
-      <c r="AC74" s="50"/>
-      <c r="AD74" s="50"/>
-      <c r="AE74" s="50"/>
-      <c r="AF74" s="50"/>
-      <c r="AG74" s="50"/>
-      <c r="AH74" s="50"/>
-      <c r="AI74" s="50"/>
-      <c r="AJ74" s="52"/>
-      <c r="AK74" s="30"/>
-      <c r="AL74" s="13"/>
-      <c r="AM74" s="13"/>
-      <c r="AN74" s="13"/>
-      <c r="AO74" s="13"/>
-      <c r="AP74" s="14"/>
+      <c r="AA74" s="24"/>
+      <c r="AB74" s="24"/>
+      <c r="AC74" s="24"/>
+      <c r="AD74" s="24"/>
+      <c r="AE74" s="24"/>
+      <c r="AF74" s="24"/>
+      <c r="AG74" s="24"/>
+      <c r="AH74" s="24"/>
+      <c r="AI74" s="24"/>
+      <c r="AJ74" s="25"/>
+      <c r="AK74" s="9"/>
+      <c r="AL74" s="10"/>
+      <c r="AM74" s="10"/>
+      <c r="AN74" s="10"/>
+      <c r="AO74" s="10"/>
+      <c r="AP74" s="11"/>
     </row>
     <row r="75" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B75" s="23" t="s">
+      <c r="B75" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="70"/>
       <c r="R75" s="4">
         <v>16</v>
       </c>
-      <c r="S75" s="49" t="s">
+      <c r="S75" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="T75" s="50"/>
-      <c r="U75" s="50"/>
-      <c r="V75" s="52"/>
-      <c r="W75" s="76" t="s">
+      <c r="T75" s="24"/>
+      <c r="U75" s="24"/>
+      <c r="V75" s="25"/>
+      <c r="W75" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="X75" s="47"/>
-      <c r="Y75" s="78"/>
-      <c r="Z75" s="51" t="s">
+      <c r="X75" s="27"/>
+      <c r="Y75" s="28"/>
+      <c r="Z75" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="AA75" s="50"/>
-      <c r="AB75" s="50"/>
-      <c r="AC75" s="50"/>
-      <c r="AD75" s="50"/>
-      <c r="AE75" s="50"/>
-      <c r="AF75" s="50"/>
-      <c r="AG75" s="50"/>
-      <c r="AH75" s="50"/>
-      <c r="AI75" s="50"/>
-      <c r="AJ75" s="52"/>
-      <c r="AK75" s="30"/>
-      <c r="AL75" s="13"/>
-      <c r="AM75" s="13"/>
-      <c r="AN75" s="13"/>
-      <c r="AO75" s="13"/>
-      <c r="AP75" s="14"/>
+      <c r="AA75" s="24"/>
+      <c r="AB75" s="24"/>
+      <c r="AC75" s="24"/>
+      <c r="AD75" s="24"/>
+      <c r="AE75" s="24"/>
+      <c r="AF75" s="24"/>
+      <c r="AG75" s="24"/>
+      <c r="AH75" s="24"/>
+      <c r="AI75" s="24"/>
+      <c r="AJ75" s="25"/>
+      <c r="AK75" s="9"/>
+      <c r="AL75" s="10"/>
+      <c r="AM75" s="10"/>
+      <c r="AN75" s="10"/>
+      <c r="AO75" s="10"/>
+      <c r="AP75" s="11"/>
     </row>
     <row r="76" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B76" s="24" t="s">
+      <c r="B76" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="24"/>
-      <c r="D76" s="24"/>
+      <c r="C76" s="71"/>
+      <c r="D76" s="71"/>
       <c r="R76" s="4">
         <v>17</v>
       </c>
-      <c r="S76" s="59" t="s">
+      <c r="S76" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="T76" s="60"/>
-      <c r="U76" s="60"/>
-      <c r="V76" s="63"/>
-      <c r="W76" s="86" t="s">
+      <c r="T76" s="64"/>
+      <c r="U76" s="64"/>
+      <c r="V76" s="65"/>
+      <c r="W76" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="X76" s="61"/>
-      <c r="Y76" s="83"/>
-      <c r="Z76" s="62" t="s">
+      <c r="X76" s="68"/>
+      <c r="Y76" s="69"/>
+      <c r="Z76" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="AA76" s="60"/>
-      <c r="AB76" s="60"/>
-      <c r="AC76" s="60"/>
-      <c r="AD76" s="60"/>
-      <c r="AE76" s="60"/>
-      <c r="AF76" s="60"/>
-      <c r="AG76" s="60"/>
-      <c r="AH76" s="60"/>
-      <c r="AI76" s="60"/>
-      <c r="AJ76" s="63"/>
-      <c r="AK76" s="88"/>
-      <c r="AL76" s="64"/>
-      <c r="AM76" s="64"/>
-      <c r="AN76" s="64"/>
-      <c r="AO76" s="64"/>
-      <c r="AP76" s="65"/>
+      <c r="AA76" s="64"/>
+      <c r="AB76" s="64"/>
+      <c r="AC76" s="64"/>
+      <c r="AD76" s="64"/>
+      <c r="AE76" s="64"/>
+      <c r="AF76" s="64"/>
+      <c r="AG76" s="64"/>
+      <c r="AH76" s="64"/>
+      <c r="AI76" s="64"/>
+      <c r="AJ76" s="65"/>
+      <c r="AK76" s="82"/>
+      <c r="AL76" s="83"/>
+      <c r="AM76" s="83"/>
+      <c r="AN76" s="83"/>
+      <c r="AO76" s="83"/>
+      <c r="AP76" s="84"/>
     </row>
     <row r="77" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="R77" s="74">
+      <c r="R77" s="6">
         <v>18</v>
       </c>
-      <c r="S77" s="49" t="s">
+      <c r="S77" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="T77" s="50"/>
-      <c r="U77" s="50"/>
-      <c r="V77" s="52"/>
-      <c r="W77" s="76" t="s">
+      <c r="T77" s="24"/>
+      <c r="U77" s="24"/>
+      <c r="V77" s="25"/>
+      <c r="W77" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="X77" s="47"/>
-      <c r="Y77" s="78"/>
-      <c r="Z77" s="51" t="s">
+      <c r="X77" s="27"/>
+      <c r="Y77" s="28"/>
+      <c r="Z77" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="AA77" s="50"/>
-      <c r="AB77" s="50"/>
-      <c r="AC77" s="50"/>
-      <c r="AD77" s="50"/>
-      <c r="AE77" s="50"/>
-      <c r="AF77" s="50"/>
-      <c r="AG77" s="50"/>
-      <c r="AH77" s="50"/>
-      <c r="AI77" s="50"/>
-      <c r="AJ77" s="52"/>
-      <c r="AK77" s="30"/>
-      <c r="AL77" s="13"/>
-      <c r="AM77" s="13"/>
-      <c r="AN77" s="13"/>
-      <c r="AO77" s="13"/>
-      <c r="AP77" s="14"/>
+      <c r="AA77" s="24"/>
+      <c r="AB77" s="24"/>
+      <c r="AC77" s="24"/>
+      <c r="AD77" s="24"/>
+      <c r="AE77" s="24"/>
+      <c r="AF77" s="24"/>
+      <c r="AG77" s="24"/>
+      <c r="AH77" s="24"/>
+      <c r="AI77" s="24"/>
+      <c r="AJ77" s="25"/>
+      <c r="AK77" s="9"/>
+      <c r="AL77" s="10"/>
+      <c r="AM77" s="10"/>
+      <c r="AN77" s="10"/>
+      <c r="AO77" s="10"/>
+      <c r="AP77" s="11"/>
     </row>
     <row r="78" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R78" s="75">
+      <c r="R78" s="7">
         <v>19</v>
       </c>
-      <c r="S78" s="53"/>
-      <c r="T78" s="54"/>
-      <c r="U78" s="54"/>
-      <c r="V78" s="56"/>
-      <c r="W78" s="77"/>
-      <c r="X78" s="55"/>
-      <c r="Y78" s="79"/>
-      <c r="Z78" s="58"/>
-      <c r="AA78" s="54"/>
-      <c r="AB78" s="54"/>
-      <c r="AC78" s="54"/>
-      <c r="AD78" s="54"/>
-      <c r="AE78" s="54"/>
-      <c r="AF78" s="54"/>
-      <c r="AG78" s="54"/>
-      <c r="AH78" s="54"/>
-      <c r="AI78" s="54"/>
-      <c r="AJ78" s="56"/>
-      <c r="AK78" s="28"/>
-      <c r="AL78" s="16"/>
-      <c r="AM78" s="16"/>
-      <c r="AN78" s="16"/>
-      <c r="AO78" s="16"/>
-      <c r="AP78" s="17"/>
+      <c r="S78" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="T78" s="13"/>
+      <c r="U78" s="13"/>
+      <c r="V78" s="14"/>
+      <c r="W78" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="X78" s="16"/>
+      <c r="Y78" s="17"/>
+      <c r="Z78" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA78" s="13"/>
+      <c r="AB78" s="13"/>
+      <c r="AC78" s="13"/>
+      <c r="AD78" s="13"/>
+      <c r="AE78" s="13"/>
+      <c r="AF78" s="13"/>
+      <c r="AG78" s="13"/>
+      <c r="AH78" s="13"/>
+      <c r="AI78" s="13"/>
+      <c r="AJ78" s="14"/>
+      <c r="AK78" s="19"/>
+      <c r="AL78" s="20"/>
+      <c r="AM78" s="20"/>
+      <c r="AN78" s="20"/>
+      <c r="AO78" s="20"/>
+      <c r="AP78" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="105">
-    <mergeCell ref="AK77:AP77"/>
-    <mergeCell ref="S78:V78"/>
-    <mergeCell ref="W78:Y78"/>
-    <mergeCell ref="Z78:AJ78"/>
-    <mergeCell ref="AK78:AP78"/>
-    <mergeCell ref="P42:T42"/>
-    <mergeCell ref="P43:T43"/>
-    <mergeCell ref="S77:V77"/>
-    <mergeCell ref="W77:Y77"/>
-    <mergeCell ref="Z77:AJ77"/>
-    <mergeCell ref="AQ14:AZ14"/>
-    <mergeCell ref="AQ15:AZ15"/>
-    <mergeCell ref="W7:AA7"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="P41:T41"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="F62:P62"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="F63:P63"/>
-    <mergeCell ref="B57:P58"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="F59:P59"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="F60:P60"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="F64:P64"/>
-    <mergeCell ref="S59:V59"/>
-    <mergeCell ref="Z59:AJ59"/>
-    <mergeCell ref="S60:V60"/>
-    <mergeCell ref="Z60:AJ60"/>
-    <mergeCell ref="S61:V61"/>
-    <mergeCell ref="Z61:AJ61"/>
-    <mergeCell ref="S62:V62"/>
-    <mergeCell ref="Z62:AJ62"/>
-    <mergeCell ref="S63:V63"/>
-    <mergeCell ref="Z63:AJ63"/>
-    <mergeCell ref="S64:V64"/>
-    <mergeCell ref="Z64:AJ64"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="F61:P61"/>
-    <mergeCell ref="S65:V65"/>
-    <mergeCell ref="Z65:AJ65"/>
-    <mergeCell ref="S66:V66"/>
-    <mergeCell ref="Z66:AJ66"/>
-    <mergeCell ref="S67:V67"/>
-    <mergeCell ref="Z67:AJ67"/>
-    <mergeCell ref="S68:V68"/>
-    <mergeCell ref="Z68:AJ68"/>
-    <mergeCell ref="S69:V69"/>
-    <mergeCell ref="Z69:AJ69"/>
-    <mergeCell ref="S70:V70"/>
-    <mergeCell ref="Z70:AJ70"/>
-    <mergeCell ref="W70:Y70"/>
-    <mergeCell ref="Z75:AJ75"/>
+    <mergeCell ref="AK75:AP75"/>
+    <mergeCell ref="AK76:AP76"/>
+    <mergeCell ref="F74:M74"/>
+    <mergeCell ref="W59:Y59"/>
+    <mergeCell ref="W60:Y60"/>
+    <mergeCell ref="W61:Y61"/>
+    <mergeCell ref="W62:Y62"/>
+    <mergeCell ref="W63:Y63"/>
+    <mergeCell ref="W64:Y64"/>
+    <mergeCell ref="W65:Y65"/>
+    <mergeCell ref="W66:Y66"/>
+    <mergeCell ref="W67:Y67"/>
+    <mergeCell ref="W68:Y68"/>
+    <mergeCell ref="W69:Y69"/>
+    <mergeCell ref="AK70:AP70"/>
+    <mergeCell ref="AK74:AP74"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="S71:V71"/>
+    <mergeCell ref="Z71:AJ71"/>
+    <mergeCell ref="S72:V72"/>
+    <mergeCell ref="Z72:AJ72"/>
+    <mergeCell ref="S73:V73"/>
+    <mergeCell ref="Z73:AJ73"/>
+    <mergeCell ref="W71:Y71"/>
+    <mergeCell ref="W72:Y72"/>
+    <mergeCell ref="W73:Y73"/>
     <mergeCell ref="S76:V76"/>
     <mergeCell ref="Z76:AJ76"/>
     <mergeCell ref="W74:Y74"/>
@@ -3215,33 +3216,61 @@
     <mergeCell ref="AK71:AP71"/>
     <mergeCell ref="AK72:AP72"/>
     <mergeCell ref="AK73:AP73"/>
-    <mergeCell ref="AK74:AP74"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="S71:V71"/>
-    <mergeCell ref="Z71:AJ71"/>
-    <mergeCell ref="S72:V72"/>
-    <mergeCell ref="Z72:AJ72"/>
-    <mergeCell ref="S73:V73"/>
-    <mergeCell ref="Z73:AJ73"/>
-    <mergeCell ref="W71:Y71"/>
-    <mergeCell ref="W72:Y72"/>
-    <mergeCell ref="W73:Y73"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="F64:P64"/>
+    <mergeCell ref="S59:V59"/>
+    <mergeCell ref="Z59:AJ59"/>
+    <mergeCell ref="S60:V60"/>
+    <mergeCell ref="Z60:AJ60"/>
+    <mergeCell ref="S61:V61"/>
+    <mergeCell ref="Z61:AJ61"/>
+    <mergeCell ref="S62:V62"/>
+    <mergeCell ref="Z62:AJ62"/>
+    <mergeCell ref="S63:V63"/>
+    <mergeCell ref="Z63:AJ63"/>
+    <mergeCell ref="S64:V64"/>
+    <mergeCell ref="Z64:AJ64"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="F61:P61"/>
+    <mergeCell ref="AQ14:AZ14"/>
+    <mergeCell ref="AQ15:AZ15"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="P41:T41"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="F62:P62"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="F63:P63"/>
+    <mergeCell ref="B57:P58"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="F59:P59"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="F60:P60"/>
     <mergeCell ref="R57:AP58"/>
-    <mergeCell ref="AK75:AP75"/>
-    <mergeCell ref="AK76:AP76"/>
-    <mergeCell ref="F74:M74"/>
-    <mergeCell ref="W59:Y59"/>
-    <mergeCell ref="W60:Y60"/>
-    <mergeCell ref="W61:Y61"/>
-    <mergeCell ref="W62:Y62"/>
-    <mergeCell ref="W63:Y63"/>
-    <mergeCell ref="W64:Y64"/>
-    <mergeCell ref="W65:Y65"/>
-    <mergeCell ref="W66:Y66"/>
-    <mergeCell ref="W67:Y67"/>
-    <mergeCell ref="W68:Y68"/>
-    <mergeCell ref="W69:Y69"/>
-    <mergeCell ref="AK70:AP70"/>
+    <mergeCell ref="AK77:AP77"/>
+    <mergeCell ref="S78:V78"/>
+    <mergeCell ref="W78:Y78"/>
+    <mergeCell ref="Z78:AJ78"/>
+    <mergeCell ref="AK78:AP78"/>
+    <mergeCell ref="P42:T42"/>
+    <mergeCell ref="P43:T43"/>
+    <mergeCell ref="S77:V77"/>
+    <mergeCell ref="W77:Y77"/>
+    <mergeCell ref="Z77:AJ77"/>
+    <mergeCell ref="S65:V65"/>
+    <mergeCell ref="Z65:AJ65"/>
+    <mergeCell ref="S66:V66"/>
+    <mergeCell ref="Z66:AJ66"/>
+    <mergeCell ref="S67:V67"/>
+    <mergeCell ref="Z67:AJ67"/>
+    <mergeCell ref="S68:V68"/>
+    <mergeCell ref="Z68:AJ68"/>
+    <mergeCell ref="S69:V69"/>
+    <mergeCell ref="Z69:AJ69"/>
+    <mergeCell ref="S70:V70"/>
+    <mergeCell ref="Z70:AJ70"/>
+    <mergeCell ref="W70:Y70"/>
+    <mergeCell ref="Z75:AJ75"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -3266,9 +3295,10 @@
     <hyperlink ref="Z75" r:id="rId19" xr:uid="{5B6689C2-94A1-4DA1-B555-A0A3093294A7}"/>
     <hyperlink ref="Z76" r:id="rId20" xr:uid="{0D8BF253-40C3-4640-804E-9611FDAAB20A}"/>
     <hyperlink ref="Z77" r:id="rId21" xr:uid="{454C94D8-4DC6-49CD-A410-D42FAF10EB15}"/>
+    <hyperlink ref="Z78" r:id="rId22" xr:uid="{995ED0EF-32F2-4DB4-B039-4E3822903D88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
-  <drawing r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
+  <drawing r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add part of the 3rd chapter
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\university\Diploma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70922965-E624-4FE3-9C50-1D28B135611F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B4501B-49B9-4CD7-82BC-F58B8A93493B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49E8A915-5A6F-4B3C-966A-272F8EBD50DB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="103">
   <si>
     <t>https://belchip.by/product/?selected_product=36951</t>
   </si>
@@ -331,6 +331,18 @@
   </si>
   <si>
     <t>https://jlcpcb.com/partdetail/Walsin_TechCorp-WR20X1001FTL/C335021</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/utc_unisonic_tech-LM2940L_50_TN3R/C85225</t>
+  </si>
+  <si>
+    <t>LM2940L-50-TN3-R</t>
+  </si>
+  <si>
+    <t>входное напряжение минимальное - 7.5, при двух батареях будет 7,4</t>
+  </si>
+  <si>
+    <t>нормальное входное напряжение (6V)</t>
   </si>
 </sst>
 </file>
@@ -411,7 +423,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -724,11 +736,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -740,19 +754,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -768,7 +769,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -780,78 +781,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -903,69 +839,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -977,7 +850,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -986,268 +859,177 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="26" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="27" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="28" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1928,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9202B416-C4F8-4CD1-A856-CE2988DE9FEF}">
-  <dimension ref="B1:AZ78"/>
+  <dimension ref="B1:AZ79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W78" sqref="W78:Y78"/>
+      <selection activeCell="AK80" sqref="AK80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,13 +1845,13 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
-      <c r="W7" s="30" t="s">
+      <c r="W7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X7" s="30"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="30"/>
-      <c r="AA7" s="30"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
     </row>
     <row r="8" spans="2:52" x14ac:dyDescent="0.25">
       <c r="G8" s="3"/>
@@ -2097,11 +1879,11 @@
       </c>
     </row>
     <row r="12" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="Q12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2129,18 +1911,18 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
-      <c r="AQ14" s="22" t="s">
+      <c r="AQ14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AR14" s="22"/>
-      <c r="AS14" s="22"/>
-      <c r="AT14" s="22"/>
-      <c r="AU14" s="22"/>
-      <c r="AV14" s="22"/>
-      <c r="AW14" s="22"/>
-      <c r="AX14" s="22"/>
-      <c r="AY14" s="22"/>
-      <c r="AZ14" s="22"/>
+      <c r="AR14" s="8"/>
+      <c r="AS14" s="8"/>
+      <c r="AT14" s="8"/>
+      <c r="AU14" s="8"/>
+      <c r="AV14" s="8"/>
+      <c r="AW14" s="8"/>
+      <c r="AX14" s="8"/>
+      <c r="AY14" s="8"/>
+      <c r="AZ14" s="8"/>
     </row>
     <row r="15" spans="2:52" x14ac:dyDescent="0.25">
       <c r="Q15" s="1"/>
@@ -2149,18 +1931,18 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
-      <c r="AQ15" s="22" t="s">
+      <c r="AQ15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AR15" s="22"/>
-      <c r="AS15" s="22"/>
-      <c r="AT15" s="22"/>
-      <c r="AU15" s="22"/>
-      <c r="AV15" s="22"/>
-      <c r="AW15" s="22"/>
-      <c r="AX15" s="22"/>
-      <c r="AY15" s="22"/>
-      <c r="AZ15" s="22"/>
+      <c r="AR15" s="8"/>
+      <c r="AS15" s="8"/>
+      <c r="AT15" s="8"/>
+      <c r="AU15" s="8"/>
+      <c r="AV15" s="8"/>
+      <c r="AW15" s="8"/>
+      <c r="AX15" s="8"/>
+      <c r="AY15" s="8"/>
+      <c r="AZ15" s="8"/>
     </row>
     <row r="16" spans="2:52" x14ac:dyDescent="0.25">
       <c r="Q16" s="1"/>
@@ -2182,13 +1964,13 @@
       <c r="B41" t="s">
         <v>14</v>
       </c>
-      <c r="P41" s="22" t="s">
+      <c r="P41" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="Q41" s="22"/>
-      <c r="R41" s="22"/>
-      <c r="S41" s="22"/>
-      <c r="T41" s="22"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
       <c r="U41" t="s">
         <v>15</v>
       </c>
@@ -2200,23 +1982,23 @@
       <c r="J42" t="s">
         <v>25</v>
       </c>
-      <c r="P42" s="22" t="s">
+      <c r="P42" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="Q42" s="22"/>
-      <c r="R42" s="22"/>
-      <c r="S42" s="22"/>
-      <c r="T42" s="22"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
       <c r="U42" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="P43" s="22"/>
-      <c r="Q43" s="22"/>
-      <c r="R43" s="22"/>
-      <c r="S43" s="22"/>
-      <c r="T43" s="22"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
@@ -2299,31 +2081,31 @@
       <c r="N58" s="37"/>
       <c r="O58" s="37"/>
       <c r="P58" s="38"/>
-      <c r="R58" s="79"/>
-      <c r="S58" s="80"/>
-      <c r="T58" s="80"/>
-      <c r="U58" s="80"/>
-      <c r="V58" s="80"/>
-      <c r="W58" s="80"/>
-      <c r="X58" s="80"/>
-      <c r="Y58" s="80"/>
-      <c r="Z58" s="80"/>
-      <c r="AA58" s="80"/>
-      <c r="AB58" s="80"/>
-      <c r="AC58" s="80"/>
-      <c r="AD58" s="80"/>
-      <c r="AE58" s="80"/>
-      <c r="AF58" s="80"/>
-      <c r="AG58" s="80"/>
-      <c r="AH58" s="80"/>
-      <c r="AI58" s="80"/>
-      <c r="AJ58" s="80"/>
-      <c r="AK58" s="80"/>
-      <c r="AL58" s="80"/>
-      <c r="AM58" s="80"/>
-      <c r="AN58" s="80"/>
-      <c r="AO58" s="80"/>
-      <c r="AP58" s="81"/>
+      <c r="R58" s="49"/>
+      <c r="S58" s="50"/>
+      <c r="T58" s="50"/>
+      <c r="U58" s="50"/>
+      <c r="V58" s="50"/>
+      <c r="W58" s="50"/>
+      <c r="X58" s="50"/>
+      <c r="Y58" s="50"/>
+      <c r="Z58" s="50"/>
+      <c r="AA58" s="50"/>
+      <c r="AB58" s="50"/>
+      <c r="AC58" s="50"/>
+      <c r="AD58" s="50"/>
+      <c r="AE58" s="50"/>
+      <c r="AF58" s="50"/>
+      <c r="AG58" s="50"/>
+      <c r="AH58" s="50"/>
+      <c r="AI58" s="50"/>
+      <c r="AJ58" s="50"/>
+      <c r="AK58" s="50"/>
+      <c r="AL58" s="50"/>
+      <c r="AM58" s="50"/>
+      <c r="AN58" s="50"/>
+      <c r="AO58" s="50"/>
+      <c r="AP58" s="51"/>
     </row>
     <row r="59" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="39" t="s">
@@ -2345,41 +2127,41 @@
       <c r="N59" s="40"/>
       <c r="O59" s="40"/>
       <c r="P59" s="41"/>
-      <c r="R59" s="5" t="s">
+      <c r="R59" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="S59" s="50" t="s">
+      <c r="S59" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="T59" s="51"/>
-      <c r="U59" s="51"/>
-      <c r="V59" s="52"/>
-      <c r="W59" s="85" t="s">
+      <c r="T59" s="19"/>
+      <c r="U59" s="19"/>
+      <c r="V59" s="27"/>
+      <c r="W59" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="X59" s="86"/>
-      <c r="Y59" s="87"/>
-      <c r="Z59" s="53" t="s">
+      <c r="X59" s="10"/>
+      <c r="Y59" s="11"/>
+      <c r="Z59" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AA59" s="51"/>
-      <c r="AB59" s="51"/>
-      <c r="AC59" s="51"/>
-      <c r="AD59" s="51"/>
-      <c r="AE59" s="51"/>
-      <c r="AF59" s="51"/>
-      <c r="AG59" s="51"/>
-      <c r="AH59" s="51"/>
-      <c r="AI59" s="51"/>
-      <c r="AJ59" s="52"/>
-      <c r="AK59" s="50" t="s">
+      <c r="AA59" s="19"/>
+      <c r="AB59" s="19"/>
+      <c r="AC59" s="19"/>
+      <c r="AD59" s="19"/>
+      <c r="AE59" s="19"/>
+      <c r="AF59" s="19"/>
+      <c r="AG59" s="19"/>
+      <c r="AH59" s="19"/>
+      <c r="AI59" s="19"/>
+      <c r="AJ59" s="27"/>
+      <c r="AK59" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="AL59" s="51"/>
-      <c r="AM59" s="51"/>
-      <c r="AN59" s="51"/>
-      <c r="AO59" s="51"/>
-      <c r="AP59" s="72"/>
+      <c r="AL59" s="19"/>
+      <c r="AM59" s="19"/>
+      <c r="AN59" s="19"/>
+      <c r="AO59" s="19"/>
+      <c r="AP59" s="20"/>
     </row>
     <row r="60" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B60" s="43" t="s">
@@ -2401,802 +2183,860 @@
       <c r="N60" s="47"/>
       <c r="O60" s="47"/>
       <c r="P60" s="48"/>
-      <c r="R60" s="8">
+      <c r="R60" s="58">
         <v>1</v>
       </c>
-      <c r="S60" s="54" t="s">
+      <c r="S60" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="T60" s="55"/>
-      <c r="U60" s="55"/>
-      <c r="V60" s="56"/>
-      <c r="W60" s="88" t="s">
+      <c r="T60" s="29"/>
+      <c r="U60" s="29"/>
+      <c r="V60" s="29"/>
+      <c r="W60" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="X60" s="89"/>
-      <c r="Y60" s="90"/>
-      <c r="Z60" s="54" t="s">
+      <c r="X60" s="12"/>
+      <c r="Y60" s="12"/>
+      <c r="Z60" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="AA60" s="55"/>
-      <c r="AB60" s="55"/>
-      <c r="AC60" s="55"/>
-      <c r="AD60" s="55"/>
-      <c r="AE60" s="55"/>
-      <c r="AF60" s="55"/>
-      <c r="AG60" s="55"/>
-      <c r="AH60" s="55"/>
-      <c r="AI60" s="55"/>
-      <c r="AJ60" s="56"/>
-      <c r="AK60" s="73" t="s">
+      <c r="AA60" s="29"/>
+      <c r="AB60" s="29"/>
+      <c r="AC60" s="29"/>
+      <c r="AD60" s="29"/>
+      <c r="AE60" s="29"/>
+      <c r="AF60" s="29"/>
+      <c r="AG60" s="29"/>
+      <c r="AH60" s="29"/>
+      <c r="AI60" s="29"/>
+      <c r="AJ60" s="29"/>
+      <c r="AK60" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="AL60" s="74"/>
-      <c r="AM60" s="74"/>
-      <c r="AN60" s="74"/>
-      <c r="AO60" s="74"/>
-      <c r="AP60" s="75"/>
+      <c r="AL60" s="21"/>
+      <c r="AM60" s="21"/>
+      <c r="AN60" s="21"/>
+      <c r="AO60" s="21"/>
+      <c r="AP60" s="22"/>
     </row>
     <row r="61" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B61" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="11"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="7"/>
       <c r="F61" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="10"/>
-      <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
-      <c r="L61" s="10"/>
-      <c r="M61" s="10"/>
-      <c r="N61" s="10"/>
-      <c r="O61" s="10"/>
-      <c r="P61" s="11"/>
-      <c r="R61" s="4">
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="6"/>
+      <c r="P61" s="7"/>
+      <c r="R61" s="59">
         <v>2</v>
       </c>
-      <c r="S61" s="57" t="s">
+      <c r="S61" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="T61" s="58"/>
-      <c r="U61" s="58"/>
-      <c r="V61" s="59"/>
-      <c r="W61" s="26" t="s">
+      <c r="T61" s="30"/>
+      <c r="U61" s="30"/>
+      <c r="V61" s="30"/>
+      <c r="W61" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="X61" s="27"/>
-      <c r="Y61" s="28"/>
-      <c r="Z61" s="57" t="s">
+      <c r="X61" s="13"/>
+      <c r="Y61" s="13"/>
+      <c r="Z61" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="AA61" s="58"/>
-      <c r="AB61" s="58"/>
-      <c r="AC61" s="58"/>
-      <c r="AD61" s="58"/>
-      <c r="AE61" s="58"/>
-      <c r="AF61" s="58"/>
-      <c r="AG61" s="58"/>
-      <c r="AH61" s="58"/>
-      <c r="AI61" s="58"/>
-      <c r="AJ61" s="59"/>
-      <c r="AK61" s="9" t="s">
+      <c r="AA61" s="30"/>
+      <c r="AB61" s="30"/>
+      <c r="AC61" s="30"/>
+      <c r="AD61" s="30"/>
+      <c r="AE61" s="30"/>
+      <c r="AF61" s="30"/>
+      <c r="AG61" s="30"/>
+      <c r="AH61" s="30"/>
+      <c r="AI61" s="30"/>
+      <c r="AJ61" s="30"/>
+      <c r="AK61" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AL61" s="10"/>
-      <c r="AM61" s="10"/>
-      <c r="AN61" s="10"/>
-      <c r="AO61" s="10"/>
-      <c r="AP61" s="11"/>
+      <c r="AL61" s="6"/>
+      <c r="AM61" s="6"/>
+      <c r="AN61" s="6"/>
+      <c r="AO61" s="6"/>
+      <c r="AP61" s="7"/>
     </row>
     <row r="62" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B62" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="11"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="7"/>
       <c r="F62" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
-      <c r="I62" s="10"/>
-      <c r="J62" s="10"/>
-      <c r="K62" s="10"/>
-      <c r="L62" s="10"/>
-      <c r="M62" s="10"/>
-      <c r="N62" s="10"/>
-      <c r="O62" s="10"/>
-      <c r="P62" s="11"/>
-      <c r="R62" s="4">
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="6"/>
+      <c r="O62" s="6"/>
+      <c r="P62" s="7"/>
+      <c r="R62" s="59">
         <v>3</v>
       </c>
-      <c r="S62" s="57" t="s">
+      <c r="S62" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="T62" s="58"/>
-      <c r="U62" s="58"/>
-      <c r="V62" s="59"/>
-      <c r="W62" s="26" t="s">
+      <c r="T62" s="30"/>
+      <c r="U62" s="30"/>
+      <c r="V62" s="30"/>
+      <c r="W62" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="X62" s="27"/>
-      <c r="Y62" s="28"/>
-      <c r="Z62" s="57" t="s">
+      <c r="X62" s="13"/>
+      <c r="Y62" s="13"/>
+      <c r="Z62" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="AA62" s="58"/>
-      <c r="AB62" s="58"/>
-      <c r="AC62" s="58"/>
-      <c r="AD62" s="58"/>
-      <c r="AE62" s="58"/>
-      <c r="AF62" s="58"/>
-      <c r="AG62" s="58"/>
-      <c r="AH62" s="58"/>
-      <c r="AI62" s="58"/>
-      <c r="AJ62" s="59"/>
-      <c r="AK62" s="9"/>
-      <c r="AL62" s="10"/>
-      <c r="AM62" s="10"/>
-      <c r="AN62" s="10"/>
-      <c r="AO62" s="10"/>
-      <c r="AP62" s="11"/>
+      <c r="AA62" s="30"/>
+      <c r="AB62" s="30"/>
+      <c r="AC62" s="30"/>
+      <c r="AD62" s="30"/>
+      <c r="AE62" s="30"/>
+      <c r="AF62" s="30"/>
+      <c r="AG62" s="30"/>
+      <c r="AH62" s="30"/>
+      <c r="AI62" s="30"/>
+      <c r="AJ62" s="30"/>
+      <c r="AK62" s="6"/>
+      <c r="AL62" s="6"/>
+      <c r="AM62" s="6"/>
+      <c r="AN62" s="6"/>
+      <c r="AO62" s="6"/>
+      <c r="AP62" s="7"/>
     </row>
     <row r="63" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B63" s="31"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
-      <c r="K63" s="10"/>
-      <c r="L63" s="10"/>
-      <c r="M63" s="10"/>
-      <c r="N63" s="10"/>
-      <c r="O63" s="10"/>
-      <c r="P63" s="11"/>
-      <c r="R63" s="4">
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="7"/>
+      <c r="R63" s="59">
         <v>4</v>
       </c>
-      <c r="S63" s="60" t="s">
+      <c r="S63" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="T63" s="61"/>
-      <c r="U63" s="61"/>
-      <c r="V63" s="62"/>
-      <c r="W63" s="26" t="s">
+      <c r="T63" s="55"/>
+      <c r="U63" s="55"/>
+      <c r="V63" s="55"/>
+      <c r="W63" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="X63" s="27"/>
-      <c r="Y63" s="28"/>
-      <c r="Z63" s="57" t="s">
+      <c r="X63" s="13"/>
+      <c r="Y63" s="13"/>
+      <c r="Z63" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="AA63" s="58"/>
-      <c r="AB63" s="58"/>
-      <c r="AC63" s="58"/>
-      <c r="AD63" s="58"/>
-      <c r="AE63" s="58"/>
-      <c r="AF63" s="58"/>
-      <c r="AG63" s="58"/>
-      <c r="AH63" s="58"/>
-      <c r="AI63" s="58"/>
-      <c r="AJ63" s="59"/>
-      <c r="AK63" s="9"/>
-      <c r="AL63" s="10"/>
-      <c r="AM63" s="10"/>
-      <c r="AN63" s="10"/>
-      <c r="AO63" s="10"/>
-      <c r="AP63" s="11"/>
+      <c r="AA63" s="30"/>
+      <c r="AB63" s="30"/>
+      <c r="AC63" s="30"/>
+      <c r="AD63" s="30"/>
+      <c r="AE63" s="30"/>
+      <c r="AF63" s="30"/>
+      <c r="AG63" s="30"/>
+      <c r="AH63" s="30"/>
+      <c r="AI63" s="30"/>
+      <c r="AJ63" s="30"/>
+      <c r="AK63" s="6"/>
+      <c r="AL63" s="6"/>
+      <c r="AM63" s="6"/>
+      <c r="AN63" s="6"/>
+      <c r="AO63" s="6"/>
+      <c r="AP63" s="7"/>
     </row>
     <row r="64" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="49"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="20"/>
-      <c r="I64" s="20"/>
-      <c r="J64" s="20"/>
-      <c r="K64" s="20"/>
-      <c r="L64" s="20"/>
-      <c r="M64" s="20"/>
-      <c r="N64" s="20"/>
-      <c r="O64" s="20"/>
-      <c r="P64" s="21"/>
-      <c r="R64" s="4">
+      <c r="B64" s="23"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="24"/>
+      <c r="H64" s="24"/>
+      <c r="I64" s="24"/>
+      <c r="J64" s="24"/>
+      <c r="K64" s="24"/>
+      <c r="L64" s="24"/>
+      <c r="M64" s="24"/>
+      <c r="N64" s="24"/>
+      <c r="O64" s="24"/>
+      <c r="P64" s="25"/>
+      <c r="R64" s="59">
         <v>5</v>
       </c>
-      <c r="S64" s="23" t="s">
+      <c r="S64" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="T64" s="24"/>
-      <c r="U64" s="24"/>
-      <c r="V64" s="25"/>
-      <c r="W64" s="26" t="s">
+      <c r="T64" s="15"/>
+      <c r="U64" s="15"/>
+      <c r="V64" s="15"/>
+      <c r="W64" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="X64" s="27"/>
-      <c r="Y64" s="28"/>
-      <c r="Z64" s="29" t="s">
+      <c r="X64" s="13"/>
+      <c r="Y64" s="13"/>
+      <c r="Z64" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="AA64" s="24"/>
-      <c r="AB64" s="24"/>
-      <c r="AC64" s="24"/>
-      <c r="AD64" s="24"/>
-      <c r="AE64" s="24"/>
-      <c r="AF64" s="24"/>
-      <c r="AG64" s="24"/>
-      <c r="AH64" s="24"/>
-      <c r="AI64" s="24"/>
-      <c r="AJ64" s="25"/>
-      <c r="AK64" s="9"/>
-      <c r="AL64" s="10"/>
-      <c r="AM64" s="10"/>
-      <c r="AN64" s="10"/>
-      <c r="AO64" s="10"/>
-      <c r="AP64" s="11"/>
+      <c r="AA64" s="15"/>
+      <c r="AB64" s="15"/>
+      <c r="AC64" s="15"/>
+      <c r="AD64" s="15"/>
+      <c r="AE64" s="15"/>
+      <c r="AF64" s="15"/>
+      <c r="AG64" s="15"/>
+      <c r="AH64" s="15"/>
+      <c r="AI64" s="15"/>
+      <c r="AJ64" s="15"/>
+      <c r="AK64" s="6"/>
+      <c r="AL64" s="6"/>
+      <c r="AM64" s="6"/>
+      <c r="AN64" s="6"/>
+      <c r="AO64" s="6"/>
+      <c r="AP64" s="7"/>
     </row>
     <row r="65" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="R65" s="4">
+      <c r="R65" s="59">
         <v>6</v>
       </c>
-      <c r="S65" s="23" t="s">
+      <c r="S65" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="T65" s="24"/>
-      <c r="U65" s="24"/>
-      <c r="V65" s="25"/>
-      <c r="W65" s="26" t="s">
+      <c r="T65" s="15"/>
+      <c r="U65" s="15"/>
+      <c r="V65" s="15"/>
+      <c r="W65" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="X65" s="27"/>
-      <c r="Y65" s="28"/>
-      <c r="Z65" s="29" t="s">
+      <c r="X65" s="13"/>
+      <c r="Y65" s="13"/>
+      <c r="Z65" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="AA65" s="24"/>
-      <c r="AB65" s="24"/>
-      <c r="AC65" s="24"/>
-      <c r="AD65" s="24"/>
-      <c r="AE65" s="24"/>
-      <c r="AF65" s="24"/>
-      <c r="AG65" s="24"/>
-      <c r="AH65" s="24"/>
-      <c r="AI65" s="24"/>
-      <c r="AJ65" s="25"/>
-      <c r="AK65" s="9"/>
-      <c r="AL65" s="10"/>
-      <c r="AM65" s="10"/>
-      <c r="AN65" s="10"/>
-      <c r="AO65" s="10"/>
-      <c r="AP65" s="11"/>
+      <c r="AA65" s="15"/>
+      <c r="AB65" s="15"/>
+      <c r="AC65" s="15"/>
+      <c r="AD65" s="15"/>
+      <c r="AE65" s="15"/>
+      <c r="AF65" s="15"/>
+      <c r="AG65" s="15"/>
+      <c r="AH65" s="15"/>
+      <c r="AI65" s="15"/>
+      <c r="AJ65" s="15"/>
+      <c r="AK65" s="6"/>
+      <c r="AL65" s="6"/>
+      <c r="AM65" s="6"/>
+      <c r="AN65" s="6"/>
+      <c r="AO65" s="6"/>
+      <c r="AP65" s="7"/>
     </row>
     <row r="66" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="R66" s="4">
+      <c r="R66" s="59">
         <v>7</v>
       </c>
-      <c r="S66" s="91" t="s">
+      <c r="S66" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="T66" s="92"/>
-      <c r="U66" s="92"/>
-      <c r="V66" s="93"/>
-      <c r="W66" s="26" t="s">
+      <c r="T66" s="54"/>
+      <c r="U66" s="54"/>
+      <c r="V66" s="54"/>
+      <c r="W66" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="X66" s="27"/>
-      <c r="Y66" s="28"/>
-      <c r="Z66" s="29" t="s">
+      <c r="X66" s="13"/>
+      <c r="Y66" s="13"/>
+      <c r="Z66" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="AA66" s="24"/>
-      <c r="AB66" s="24"/>
-      <c r="AC66" s="24"/>
-      <c r="AD66" s="24"/>
-      <c r="AE66" s="24"/>
-      <c r="AF66" s="24"/>
-      <c r="AG66" s="24"/>
-      <c r="AH66" s="24"/>
-      <c r="AI66" s="24"/>
-      <c r="AJ66" s="25"/>
-      <c r="AK66" s="9" t="s">
+      <c r="AA66" s="15"/>
+      <c r="AB66" s="15"/>
+      <c r="AC66" s="15"/>
+      <c r="AD66" s="15"/>
+      <c r="AE66" s="15"/>
+      <c r="AF66" s="15"/>
+      <c r="AG66" s="15"/>
+      <c r="AH66" s="15"/>
+      <c r="AI66" s="15"/>
+      <c r="AJ66" s="15"/>
+      <c r="AK66" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="AL66" s="10"/>
-      <c r="AM66" s="10"/>
-      <c r="AN66" s="10"/>
-      <c r="AO66" s="10"/>
-      <c r="AP66" s="11"/>
+      <c r="AL66" s="6"/>
+      <c r="AM66" s="6"/>
+      <c r="AN66" s="6"/>
+      <c r="AO66" s="6"/>
+      <c r="AP66" s="7"/>
     </row>
     <row r="67" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="R67" s="4">
+      <c r="R67" s="59">
         <v>8</v>
       </c>
-      <c r="S67" s="23" t="s">
+      <c r="S67" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T67" s="24"/>
-      <c r="U67" s="24"/>
-      <c r="V67" s="25"/>
-      <c r="W67" s="26" t="s">
+      <c r="T67" s="15"/>
+      <c r="U67" s="15"/>
+      <c r="V67" s="15"/>
+      <c r="W67" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="X67" s="27"/>
-      <c r="Y67" s="28"/>
-      <c r="Z67" s="29" t="s">
+      <c r="X67" s="13"/>
+      <c r="Y67" s="13"/>
+      <c r="Z67" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="AA67" s="24"/>
-      <c r="AB67" s="24"/>
-      <c r="AC67" s="24"/>
-      <c r="AD67" s="24"/>
-      <c r="AE67" s="24"/>
-      <c r="AF67" s="24"/>
-      <c r="AG67" s="24"/>
-      <c r="AH67" s="24"/>
-      <c r="AI67" s="24"/>
-      <c r="AJ67" s="25"/>
-      <c r="AK67" s="9"/>
-      <c r="AL67" s="10"/>
-      <c r="AM67" s="10"/>
-      <c r="AN67" s="10"/>
-      <c r="AO67" s="10"/>
-      <c r="AP67" s="11"/>
+      <c r="AA67" s="15"/>
+      <c r="AB67" s="15"/>
+      <c r="AC67" s="15"/>
+      <c r="AD67" s="15"/>
+      <c r="AE67" s="15"/>
+      <c r="AF67" s="15"/>
+      <c r="AG67" s="15"/>
+      <c r="AH67" s="15"/>
+      <c r="AI67" s="15"/>
+      <c r="AJ67" s="15"/>
+      <c r="AK67" s="6"/>
+      <c r="AL67" s="6"/>
+      <c r="AM67" s="6"/>
+      <c r="AN67" s="6"/>
+      <c r="AO67" s="6"/>
+      <c r="AP67" s="7"/>
     </row>
     <row r="68" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="R68" s="4">
+      <c r="R68" s="59">
         <v>9</v>
       </c>
-      <c r="S68" s="23" t="s">
+      <c r="S68" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="T68" s="24"/>
-      <c r="U68" s="24"/>
-      <c r="V68" s="25"/>
-      <c r="W68" s="26" t="s">
+      <c r="T68" s="15"/>
+      <c r="U68" s="15"/>
+      <c r="V68" s="15"/>
+      <c r="W68" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="X68" s="27"/>
-      <c r="Y68" s="28"/>
-      <c r="Z68" s="29" t="s">
+      <c r="X68" s="13"/>
+      <c r="Y68" s="13"/>
+      <c r="Z68" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="AA68" s="24"/>
-      <c r="AB68" s="24"/>
-      <c r="AC68" s="24"/>
-      <c r="AD68" s="24"/>
-      <c r="AE68" s="24"/>
-      <c r="AF68" s="24"/>
-      <c r="AG68" s="24"/>
-      <c r="AH68" s="24"/>
-      <c r="AI68" s="24"/>
-      <c r="AJ68" s="25"/>
-      <c r="AK68" s="9"/>
-      <c r="AL68" s="10"/>
-      <c r="AM68" s="10"/>
-      <c r="AN68" s="10"/>
-      <c r="AO68" s="10"/>
-      <c r="AP68" s="11"/>
+      <c r="AA68" s="15"/>
+      <c r="AB68" s="15"/>
+      <c r="AC68" s="15"/>
+      <c r="AD68" s="15"/>
+      <c r="AE68" s="15"/>
+      <c r="AF68" s="15"/>
+      <c r="AG68" s="15"/>
+      <c r="AH68" s="15"/>
+      <c r="AI68" s="15"/>
+      <c r="AJ68" s="15"/>
+      <c r="AK68" s="6"/>
+      <c r="AL68" s="6"/>
+      <c r="AM68" s="6"/>
+      <c r="AN68" s="6"/>
+      <c r="AO68" s="6"/>
+      <c r="AP68" s="7"/>
     </row>
     <row r="69" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="R69" s="4">
+      <c r="R69" s="59">
         <v>10</v>
       </c>
-      <c r="S69" s="23" t="s">
+      <c r="S69" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="T69" s="24"/>
-      <c r="U69" s="24"/>
-      <c r="V69" s="25"/>
-      <c r="W69" s="26" t="s">
+      <c r="T69" s="15"/>
+      <c r="U69" s="15"/>
+      <c r="V69" s="15"/>
+      <c r="W69" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="X69" s="27"/>
-      <c r="Y69" s="28"/>
-      <c r="Z69" s="29" t="s">
+      <c r="X69" s="13"/>
+      <c r="Y69" s="13"/>
+      <c r="Z69" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="AA69" s="24"/>
-      <c r="AB69" s="24"/>
-      <c r="AC69" s="24"/>
-      <c r="AD69" s="24"/>
-      <c r="AE69" s="24"/>
-      <c r="AF69" s="24"/>
-      <c r="AG69" s="24"/>
-      <c r="AH69" s="24"/>
-      <c r="AI69" s="24"/>
-      <c r="AJ69" s="25"/>
-      <c r="AK69" s="9"/>
-      <c r="AL69" s="10"/>
-      <c r="AM69" s="10"/>
-      <c r="AN69" s="10"/>
-      <c r="AO69" s="10"/>
-      <c r="AP69" s="11"/>
+      <c r="AA69" s="15"/>
+      <c r="AB69" s="15"/>
+      <c r="AC69" s="15"/>
+      <c r="AD69" s="15"/>
+      <c r="AE69" s="15"/>
+      <c r="AF69" s="15"/>
+      <c r="AG69" s="15"/>
+      <c r="AH69" s="15"/>
+      <c r="AI69" s="15"/>
+      <c r="AJ69" s="15"/>
+      <c r="AK69" s="6"/>
+      <c r="AL69" s="6"/>
+      <c r="AM69" s="6"/>
+      <c r="AN69" s="6"/>
+      <c r="AO69" s="6"/>
+      <c r="AP69" s="7"/>
     </row>
     <row r="70" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="R70" s="4">
+      <c r="R70" s="59">
         <v>11</v>
       </c>
-      <c r="S70" s="23" t="s">
+      <c r="S70" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="T70" s="24"/>
-      <c r="U70" s="24"/>
-      <c r="V70" s="25"/>
-      <c r="W70" s="26" t="s">
+      <c r="T70" s="15"/>
+      <c r="U70" s="15"/>
+      <c r="V70" s="15"/>
+      <c r="W70" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="X70" s="27"/>
-      <c r="Y70" s="28"/>
-      <c r="Z70" s="29" t="s">
+      <c r="X70" s="13"/>
+      <c r="Y70" s="13"/>
+      <c r="Z70" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="AA70" s="24"/>
-      <c r="AB70" s="24"/>
-      <c r="AC70" s="24"/>
-      <c r="AD70" s="24"/>
-      <c r="AE70" s="24"/>
-      <c r="AF70" s="24"/>
-      <c r="AG70" s="24"/>
-      <c r="AH70" s="24"/>
-      <c r="AI70" s="24"/>
-      <c r="AJ70" s="25"/>
-      <c r="AK70" s="9"/>
-      <c r="AL70" s="10"/>
-      <c r="AM70" s="10"/>
-      <c r="AN70" s="10"/>
-      <c r="AO70" s="10"/>
-      <c r="AP70" s="11"/>
+      <c r="AA70" s="15"/>
+      <c r="AB70" s="15"/>
+      <c r="AC70" s="15"/>
+      <c r="AD70" s="15"/>
+      <c r="AE70" s="15"/>
+      <c r="AF70" s="15"/>
+      <c r="AG70" s="15"/>
+      <c r="AH70" s="15"/>
+      <c r="AI70" s="15"/>
+      <c r="AJ70" s="15"/>
+      <c r="AK70" s="6"/>
+      <c r="AL70" s="6"/>
+      <c r="AM70" s="6"/>
+      <c r="AN70" s="6"/>
+      <c r="AO70" s="6"/>
+      <c r="AP70" s="7"/>
     </row>
     <row r="71" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="R71" s="4">
+      <c r="R71" s="59">
         <v>12</v>
       </c>
-      <c r="S71" s="23" t="s">
+      <c r="S71" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="T71" s="24"/>
-      <c r="U71" s="24"/>
-      <c r="V71" s="25"/>
-      <c r="W71" s="26" t="s">
+      <c r="T71" s="15"/>
+      <c r="U71" s="15"/>
+      <c r="V71" s="15"/>
+      <c r="W71" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="X71" s="27"/>
-      <c r="Y71" s="28"/>
-      <c r="Z71" s="29" t="s">
+      <c r="X71" s="13"/>
+      <c r="Y71" s="13"/>
+      <c r="Z71" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="AA71" s="24"/>
-      <c r="AB71" s="24"/>
-      <c r="AC71" s="24"/>
-      <c r="AD71" s="24"/>
-      <c r="AE71" s="24"/>
-      <c r="AF71" s="24"/>
-      <c r="AG71" s="24"/>
-      <c r="AH71" s="24"/>
-      <c r="AI71" s="24"/>
-      <c r="AJ71" s="25"/>
-      <c r="AK71" s="9"/>
-      <c r="AL71" s="10"/>
-      <c r="AM71" s="10"/>
-      <c r="AN71" s="10"/>
-      <c r="AO71" s="10"/>
-      <c r="AP71" s="11"/>
+      <c r="AA71" s="15"/>
+      <c r="AB71" s="15"/>
+      <c r="AC71" s="15"/>
+      <c r="AD71" s="15"/>
+      <c r="AE71" s="15"/>
+      <c r="AF71" s="15"/>
+      <c r="AG71" s="15"/>
+      <c r="AH71" s="15"/>
+      <c r="AI71" s="15"/>
+      <c r="AJ71" s="15"/>
+      <c r="AK71" s="6"/>
+      <c r="AL71" s="6"/>
+      <c r="AM71" s="6"/>
+      <c r="AN71" s="6"/>
+      <c r="AO71" s="6"/>
+      <c r="AP71" s="7"/>
     </row>
     <row r="72" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="R72" s="4">
+      <c r="R72" s="59">
         <v>13</v>
       </c>
-      <c r="S72" s="23" t="s">
+      <c r="S72" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="T72" s="24"/>
-      <c r="U72" s="24"/>
-      <c r="V72" s="25"/>
-      <c r="W72" s="76" t="s">
+      <c r="T72" s="15"/>
+      <c r="U72" s="15"/>
+      <c r="V72" s="15"/>
+      <c r="W72" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="X72" s="77"/>
-      <c r="Y72" s="78"/>
-      <c r="Z72" s="29" t="s">
+      <c r="X72" s="57"/>
+      <c r="Y72" s="57"/>
+      <c r="Z72" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="AA72" s="24"/>
-      <c r="AB72" s="24"/>
-      <c r="AC72" s="24"/>
-      <c r="AD72" s="24"/>
-      <c r="AE72" s="24"/>
-      <c r="AF72" s="24"/>
-      <c r="AG72" s="24"/>
-      <c r="AH72" s="24"/>
-      <c r="AI72" s="24"/>
-      <c r="AJ72" s="25"/>
-      <c r="AK72" s="9"/>
-      <c r="AL72" s="10"/>
-      <c r="AM72" s="10"/>
-      <c r="AN72" s="10"/>
-      <c r="AO72" s="10"/>
-      <c r="AP72" s="11"/>
+      <c r="AA72" s="15"/>
+      <c r="AB72" s="15"/>
+      <c r="AC72" s="15"/>
+      <c r="AD72" s="15"/>
+      <c r="AE72" s="15"/>
+      <c r="AF72" s="15"/>
+      <c r="AG72" s="15"/>
+      <c r="AH72" s="15"/>
+      <c r="AI72" s="15"/>
+      <c r="AJ72" s="15"/>
+      <c r="AK72" s="6"/>
+      <c r="AL72" s="6"/>
+      <c r="AM72" s="6"/>
+      <c r="AN72" s="6"/>
+      <c r="AO72" s="6"/>
+      <c r="AP72" s="7"/>
     </row>
     <row r="73" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="R73" s="4">
+      <c r="R73" s="59">
         <v>14</v>
       </c>
-      <c r="S73" s="23" t="s">
+      <c r="S73" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="T73" s="24"/>
-      <c r="U73" s="24"/>
-      <c r="V73" s="25"/>
-      <c r="W73" s="26" t="s">
+      <c r="T73" s="15"/>
+      <c r="U73" s="15"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="X73" s="27"/>
-      <c r="Y73" s="28"/>
-      <c r="Z73" s="29" t="s">
+      <c r="X73" s="13"/>
+      <c r="Y73" s="13"/>
+      <c r="Z73" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="AA73" s="24"/>
-      <c r="AB73" s="24"/>
-      <c r="AC73" s="24"/>
-      <c r="AD73" s="24"/>
-      <c r="AE73" s="24"/>
-      <c r="AF73" s="24"/>
-      <c r="AG73" s="24"/>
-      <c r="AH73" s="24"/>
-      <c r="AI73" s="24"/>
-      <c r="AJ73" s="25"/>
-      <c r="AK73" s="9"/>
-      <c r="AL73" s="10"/>
-      <c r="AM73" s="10"/>
-      <c r="AN73" s="10"/>
-      <c r="AO73" s="10"/>
-      <c r="AP73" s="11"/>
+      <c r="AA73" s="15"/>
+      <c r="AB73" s="15"/>
+      <c r="AC73" s="15"/>
+      <c r="AD73" s="15"/>
+      <c r="AE73" s="15"/>
+      <c r="AF73" s="15"/>
+      <c r="AG73" s="15"/>
+      <c r="AH73" s="15"/>
+      <c r="AI73" s="15"/>
+      <c r="AJ73" s="15"/>
+      <c r="AK73" s="6"/>
+      <c r="AL73" s="6"/>
+      <c r="AM73" s="6"/>
+      <c r="AN73" s="6"/>
+      <c r="AO73" s="6"/>
+      <c r="AP73" s="7"/>
     </row>
     <row r="74" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
-      <c r="F74" s="22" t="s">
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="F74" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G74" s="22"/>
-      <c r="H74" s="22"/>
-      <c r="I74" s="22"/>
-      <c r="J74" s="22"/>
-      <c r="K74" s="22"/>
-      <c r="L74" s="22"/>
-      <c r="M74" s="22"/>
-      <c r="R74" s="4">
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="8"/>
+      <c r="L74" s="8"/>
+      <c r="M74" s="8"/>
+      <c r="R74" s="59">
         <v>15</v>
       </c>
-      <c r="S74" s="23" t="s">
+      <c r="S74" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="T74" s="24"/>
-      <c r="U74" s="24"/>
-      <c r="V74" s="25"/>
-      <c r="W74" s="26" t="s">
+      <c r="T74" s="30"/>
+      <c r="U74" s="30"/>
+      <c r="V74" s="30"/>
+      <c r="W74" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="X74" s="27"/>
-      <c r="Y74" s="28"/>
-      <c r="Z74" s="29" t="s">
+      <c r="X74" s="13"/>
+      <c r="Y74" s="13"/>
+      <c r="Z74" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="AA74" s="24"/>
-      <c r="AB74" s="24"/>
-      <c r="AC74" s="24"/>
-      <c r="AD74" s="24"/>
-      <c r="AE74" s="24"/>
-      <c r="AF74" s="24"/>
-      <c r="AG74" s="24"/>
-      <c r="AH74" s="24"/>
-      <c r="AI74" s="24"/>
-      <c r="AJ74" s="25"/>
-      <c r="AK74" s="9"/>
-      <c r="AL74" s="10"/>
-      <c r="AM74" s="10"/>
-      <c r="AN74" s="10"/>
-      <c r="AO74" s="10"/>
-      <c r="AP74" s="11"/>
+      <c r="AA74" s="15"/>
+      <c r="AB74" s="15"/>
+      <c r="AC74" s="15"/>
+      <c r="AD74" s="15"/>
+      <c r="AE74" s="15"/>
+      <c r="AF74" s="15"/>
+      <c r="AG74" s="15"/>
+      <c r="AH74" s="15"/>
+      <c r="AI74" s="15"/>
+      <c r="AJ74" s="15"/>
+      <c r="AK74" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL74" s="6"/>
+      <c r="AM74" s="6"/>
+      <c r="AN74" s="6"/>
+      <c r="AO74" s="6"/>
+      <c r="AP74" s="7"/>
     </row>
     <row r="75" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B75" s="70" t="s">
+      <c r="B75" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C75" s="70"/>
-      <c r="D75" s="70"/>
-      <c r="R75" s="4">
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
+      <c r="R75" s="59">
         <v>16</v>
       </c>
-      <c r="S75" s="23" t="s">
+      <c r="S75" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="T75" s="24"/>
-      <c r="U75" s="24"/>
-      <c r="V75" s="25"/>
-      <c r="W75" s="26" t="s">
+      <c r="T75" s="15"/>
+      <c r="U75" s="15"/>
+      <c r="V75" s="15"/>
+      <c r="W75" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="X75" s="27"/>
-      <c r="Y75" s="28"/>
-      <c r="Z75" s="29" t="s">
+      <c r="X75" s="13"/>
+      <c r="Y75" s="13"/>
+      <c r="Z75" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="AA75" s="24"/>
-      <c r="AB75" s="24"/>
-      <c r="AC75" s="24"/>
-      <c r="AD75" s="24"/>
-      <c r="AE75" s="24"/>
-      <c r="AF75" s="24"/>
-      <c r="AG75" s="24"/>
-      <c r="AH75" s="24"/>
-      <c r="AI75" s="24"/>
-      <c r="AJ75" s="25"/>
-      <c r="AK75" s="9"/>
-      <c r="AL75" s="10"/>
-      <c r="AM75" s="10"/>
-      <c r="AN75" s="10"/>
-      <c r="AO75" s="10"/>
-      <c r="AP75" s="11"/>
+      <c r="AA75" s="15"/>
+      <c r="AB75" s="15"/>
+      <c r="AC75" s="15"/>
+      <c r="AD75" s="15"/>
+      <c r="AE75" s="15"/>
+      <c r="AF75" s="15"/>
+      <c r="AG75" s="15"/>
+      <c r="AH75" s="15"/>
+      <c r="AI75" s="15"/>
+      <c r="AJ75" s="15"/>
+      <c r="AK75" s="6"/>
+      <c r="AL75" s="6"/>
+      <c r="AM75" s="6"/>
+      <c r="AN75" s="6"/>
+      <c r="AO75" s="6"/>
+      <c r="AP75" s="7"/>
     </row>
     <row r="76" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B76" s="71" t="s">
+      <c r="B76" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="71"/>
-      <c r="D76" s="71"/>
-      <c r="R76" s="4">
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="R76" s="59">
         <v>17</v>
       </c>
-      <c r="S76" s="63" t="s">
+      <c r="S76" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="T76" s="64"/>
-      <c r="U76" s="64"/>
-      <c r="V76" s="65"/>
-      <c r="W76" s="67" t="s">
+      <c r="T76" s="15"/>
+      <c r="U76" s="15"/>
+      <c r="V76" s="15"/>
+      <c r="W76" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="X76" s="68"/>
-      <c r="Y76" s="69"/>
-      <c r="Z76" s="66" t="s">
+      <c r="X76" s="13"/>
+      <c r="Y76" s="13"/>
+      <c r="Z76" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="AA76" s="64"/>
-      <c r="AB76" s="64"/>
-      <c r="AC76" s="64"/>
-      <c r="AD76" s="64"/>
-      <c r="AE76" s="64"/>
-      <c r="AF76" s="64"/>
-      <c r="AG76" s="64"/>
-      <c r="AH76" s="64"/>
-      <c r="AI76" s="64"/>
-      <c r="AJ76" s="65"/>
-      <c r="AK76" s="82"/>
-      <c r="AL76" s="83"/>
-      <c r="AM76" s="83"/>
-      <c r="AN76" s="83"/>
-      <c r="AO76" s="83"/>
-      <c r="AP76" s="84"/>
+      <c r="AA76" s="15"/>
+      <c r="AB76" s="15"/>
+      <c r="AC76" s="15"/>
+      <c r="AD76" s="15"/>
+      <c r="AE76" s="15"/>
+      <c r="AF76" s="15"/>
+      <c r="AG76" s="15"/>
+      <c r="AH76" s="15"/>
+      <c r="AI76" s="15"/>
+      <c r="AJ76" s="15"/>
+      <c r="AK76" s="6"/>
+      <c r="AL76" s="6"/>
+      <c r="AM76" s="6"/>
+      <c r="AN76" s="6"/>
+      <c r="AO76" s="6"/>
+      <c r="AP76" s="7"/>
     </row>
     <row r="77" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="R77" s="6">
+      <c r="R77" s="59">
         <v>18</v>
       </c>
-      <c r="S77" s="23" t="s">
+      <c r="S77" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="T77" s="24"/>
-      <c r="U77" s="24"/>
-      <c r="V77" s="25"/>
-      <c r="W77" s="26" t="s">
+      <c r="T77" s="15"/>
+      <c r="U77" s="15"/>
+      <c r="V77" s="15"/>
+      <c r="W77" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="X77" s="27"/>
-      <c r="Y77" s="28"/>
-      <c r="Z77" s="29" t="s">
+      <c r="X77" s="13"/>
+      <c r="Y77" s="13"/>
+      <c r="Z77" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="AA77" s="24"/>
-      <c r="AB77" s="24"/>
-      <c r="AC77" s="24"/>
-      <c r="AD77" s="24"/>
-      <c r="AE77" s="24"/>
-      <c r="AF77" s="24"/>
-      <c r="AG77" s="24"/>
-      <c r="AH77" s="24"/>
-      <c r="AI77" s="24"/>
-      <c r="AJ77" s="25"/>
-      <c r="AK77" s="9"/>
-      <c r="AL77" s="10"/>
-      <c r="AM77" s="10"/>
-      <c r="AN77" s="10"/>
-      <c r="AO77" s="10"/>
-      <c r="AP77" s="11"/>
-    </row>
-    <row r="78" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R78" s="7">
+      <c r="AA77" s="15"/>
+      <c r="AB77" s="15"/>
+      <c r="AC77" s="15"/>
+      <c r="AD77" s="15"/>
+      <c r="AE77" s="15"/>
+      <c r="AF77" s="15"/>
+      <c r="AG77" s="15"/>
+      <c r="AH77" s="15"/>
+      <c r="AI77" s="15"/>
+      <c r="AJ77" s="15"/>
+      <c r="AK77" s="6"/>
+      <c r="AL77" s="6"/>
+      <c r="AM77" s="6"/>
+      <c r="AN77" s="6"/>
+      <c r="AO77" s="6"/>
+      <c r="AP77" s="7"/>
+    </row>
+    <row r="78" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="R78" s="59">
         <v>19</v>
       </c>
-      <c r="S78" s="12" t="s">
+      <c r="S78" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="T78" s="13"/>
-      <c r="U78" s="13"/>
-      <c r="V78" s="14"/>
-      <c r="W78" s="15" t="s">
+      <c r="T78" s="15"/>
+      <c r="U78" s="15"/>
+      <c r="V78" s="15"/>
+      <c r="W78" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="X78" s="16"/>
-      <c r="Y78" s="17"/>
-      <c r="Z78" s="18" t="s">
+      <c r="X78" s="13"/>
+      <c r="Y78" s="13"/>
+      <c r="Z78" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="AA78" s="13"/>
-      <c r="AB78" s="13"/>
-      <c r="AC78" s="13"/>
-      <c r="AD78" s="13"/>
-      <c r="AE78" s="13"/>
-      <c r="AF78" s="13"/>
-      <c r="AG78" s="13"/>
-      <c r="AH78" s="13"/>
-      <c r="AI78" s="13"/>
-      <c r="AJ78" s="14"/>
-      <c r="AK78" s="19"/>
-      <c r="AL78" s="20"/>
-      <c r="AM78" s="20"/>
-      <c r="AN78" s="20"/>
-      <c r="AO78" s="20"/>
-      <c r="AP78" s="21"/>
+      <c r="AA78" s="15"/>
+      <c r="AB78" s="15"/>
+      <c r="AC78" s="15"/>
+      <c r="AD78" s="15"/>
+      <c r="AE78" s="15"/>
+      <c r="AF78" s="15"/>
+      <c r="AG78" s="15"/>
+      <c r="AH78" s="15"/>
+      <c r="AI78" s="15"/>
+      <c r="AJ78" s="15"/>
+      <c r="AK78" s="6"/>
+      <c r="AL78" s="6"/>
+      <c r="AM78" s="6"/>
+      <c r="AN78" s="6"/>
+      <c r="AO78" s="6"/>
+      <c r="AP78" s="7"/>
+    </row>
+    <row r="79" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R79" s="60">
+        <v>19</v>
+      </c>
+      <c r="S79" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="T79" s="61"/>
+      <c r="U79" s="61"/>
+      <c r="V79" s="61"/>
+      <c r="W79" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="X79" s="53"/>
+      <c r="Y79" s="53"/>
+      <c r="Z79" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA79" s="52"/>
+      <c r="AB79" s="52"/>
+      <c r="AC79" s="52"/>
+      <c r="AD79" s="52"/>
+      <c r="AE79" s="52"/>
+      <c r="AF79" s="52"/>
+      <c r="AG79" s="52"/>
+      <c r="AH79" s="52"/>
+      <c r="AI79" s="52"/>
+      <c r="AJ79" s="52"/>
+      <c r="AK79" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL79" s="24"/>
+      <c r="AM79" s="24"/>
+      <c r="AN79" s="24"/>
+      <c r="AO79" s="24"/>
+      <c r="AP79" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="105">
-    <mergeCell ref="AK75:AP75"/>
-    <mergeCell ref="AK76:AP76"/>
-    <mergeCell ref="F74:M74"/>
-    <mergeCell ref="W59:Y59"/>
-    <mergeCell ref="W60:Y60"/>
-    <mergeCell ref="W61:Y61"/>
-    <mergeCell ref="W62:Y62"/>
-    <mergeCell ref="W63:Y63"/>
-    <mergeCell ref="W64:Y64"/>
-    <mergeCell ref="W65:Y65"/>
-    <mergeCell ref="W66:Y66"/>
-    <mergeCell ref="W67:Y67"/>
-    <mergeCell ref="W68:Y68"/>
-    <mergeCell ref="W69:Y69"/>
-    <mergeCell ref="AK70:AP70"/>
-    <mergeCell ref="AK74:AP74"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="S71:V71"/>
-    <mergeCell ref="Z71:AJ71"/>
-    <mergeCell ref="S72:V72"/>
-    <mergeCell ref="Z72:AJ72"/>
-    <mergeCell ref="S73:V73"/>
-    <mergeCell ref="Z73:AJ73"/>
-    <mergeCell ref="W71:Y71"/>
-    <mergeCell ref="W72:Y72"/>
-    <mergeCell ref="W73:Y73"/>
-    <mergeCell ref="S76:V76"/>
-    <mergeCell ref="Z76:AJ76"/>
-    <mergeCell ref="W74:Y74"/>
-    <mergeCell ref="W75:Y75"/>
-    <mergeCell ref="W76:Y76"/>
+  <mergeCells count="109">
+    <mergeCell ref="S79:V79"/>
+    <mergeCell ref="W79:Y79"/>
+    <mergeCell ref="Z79:AJ79"/>
+    <mergeCell ref="AK79:AP79"/>
+    <mergeCell ref="AK77:AP77"/>
+    <mergeCell ref="S78:V78"/>
+    <mergeCell ref="W78:Y78"/>
+    <mergeCell ref="Z78:AJ78"/>
+    <mergeCell ref="AK78:AP78"/>
+    <mergeCell ref="P42:T42"/>
+    <mergeCell ref="P43:T43"/>
+    <mergeCell ref="S77:V77"/>
+    <mergeCell ref="W77:Y77"/>
+    <mergeCell ref="Z77:AJ77"/>
+    <mergeCell ref="S65:V65"/>
+    <mergeCell ref="Z65:AJ65"/>
+    <mergeCell ref="S66:V66"/>
+    <mergeCell ref="Z66:AJ66"/>
+    <mergeCell ref="S67:V67"/>
+    <mergeCell ref="Z67:AJ67"/>
+    <mergeCell ref="S68:V68"/>
+    <mergeCell ref="Z68:AJ68"/>
+    <mergeCell ref="S69:V69"/>
+    <mergeCell ref="Z69:AJ69"/>
+    <mergeCell ref="S70:V70"/>
+    <mergeCell ref="Z70:AJ70"/>
+    <mergeCell ref="W70:Y70"/>
+    <mergeCell ref="Z75:AJ75"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="P41:T41"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="F62:P62"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="F63:P63"/>
+    <mergeCell ref="B57:P58"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="F59:P59"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="F60:P60"/>
+    <mergeCell ref="R57:AP58"/>
+    <mergeCell ref="Z62:AJ62"/>
+    <mergeCell ref="S63:V63"/>
+    <mergeCell ref="Z63:AJ63"/>
+    <mergeCell ref="S64:V64"/>
+    <mergeCell ref="Z64:AJ64"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="F61:P61"/>
+    <mergeCell ref="AQ14:AZ14"/>
+    <mergeCell ref="AQ15:AZ15"/>
     <mergeCell ref="B75:D75"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="AK59:AP59"/>
@@ -3221,56 +3061,41 @@
     <mergeCell ref="S59:V59"/>
     <mergeCell ref="Z59:AJ59"/>
     <mergeCell ref="S60:V60"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="S71:V71"/>
+    <mergeCell ref="Z71:AJ71"/>
+    <mergeCell ref="S72:V72"/>
+    <mergeCell ref="Z72:AJ72"/>
+    <mergeCell ref="S73:V73"/>
+    <mergeCell ref="Z73:AJ73"/>
+    <mergeCell ref="W71:Y71"/>
+    <mergeCell ref="W72:Y72"/>
+    <mergeCell ref="W73:Y73"/>
+    <mergeCell ref="W74:Y74"/>
+    <mergeCell ref="AK75:AP75"/>
+    <mergeCell ref="AK76:AP76"/>
+    <mergeCell ref="F74:M74"/>
+    <mergeCell ref="W59:Y59"/>
+    <mergeCell ref="W60:Y60"/>
+    <mergeCell ref="W61:Y61"/>
+    <mergeCell ref="W62:Y62"/>
+    <mergeCell ref="W63:Y63"/>
+    <mergeCell ref="W64:Y64"/>
+    <mergeCell ref="W65:Y65"/>
+    <mergeCell ref="W66:Y66"/>
+    <mergeCell ref="W67:Y67"/>
+    <mergeCell ref="W68:Y68"/>
+    <mergeCell ref="W69:Y69"/>
+    <mergeCell ref="AK70:AP70"/>
+    <mergeCell ref="AK74:AP74"/>
+    <mergeCell ref="S76:V76"/>
+    <mergeCell ref="Z76:AJ76"/>
+    <mergeCell ref="W75:Y75"/>
+    <mergeCell ref="W76:Y76"/>
     <mergeCell ref="Z60:AJ60"/>
     <mergeCell ref="S61:V61"/>
     <mergeCell ref="Z61:AJ61"/>
     <mergeCell ref="S62:V62"/>
-    <mergeCell ref="Z62:AJ62"/>
-    <mergeCell ref="S63:V63"/>
-    <mergeCell ref="Z63:AJ63"/>
-    <mergeCell ref="S64:V64"/>
-    <mergeCell ref="Z64:AJ64"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="F61:P61"/>
-    <mergeCell ref="AQ14:AZ14"/>
-    <mergeCell ref="AQ15:AZ15"/>
-    <mergeCell ref="W7:AA7"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="P41:T41"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="F62:P62"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="F63:P63"/>
-    <mergeCell ref="B57:P58"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="F59:P59"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="F60:P60"/>
-    <mergeCell ref="R57:AP58"/>
-    <mergeCell ref="AK77:AP77"/>
-    <mergeCell ref="S78:V78"/>
-    <mergeCell ref="W78:Y78"/>
-    <mergeCell ref="Z78:AJ78"/>
-    <mergeCell ref="AK78:AP78"/>
-    <mergeCell ref="P42:T42"/>
-    <mergeCell ref="P43:T43"/>
-    <mergeCell ref="S77:V77"/>
-    <mergeCell ref="W77:Y77"/>
-    <mergeCell ref="Z77:AJ77"/>
-    <mergeCell ref="S65:V65"/>
-    <mergeCell ref="Z65:AJ65"/>
-    <mergeCell ref="S66:V66"/>
-    <mergeCell ref="Z66:AJ66"/>
-    <mergeCell ref="S67:V67"/>
-    <mergeCell ref="Z67:AJ67"/>
-    <mergeCell ref="S68:V68"/>
-    <mergeCell ref="Z68:AJ68"/>
-    <mergeCell ref="S69:V69"/>
-    <mergeCell ref="Z69:AJ69"/>
-    <mergeCell ref="S70:V70"/>
-    <mergeCell ref="Z70:AJ70"/>
-    <mergeCell ref="W70:Y70"/>
-    <mergeCell ref="Z75:AJ75"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -3296,9 +3121,10 @@
     <hyperlink ref="Z76" r:id="rId20" xr:uid="{0D8BF253-40C3-4640-804E-9611FDAAB20A}"/>
     <hyperlink ref="Z77" r:id="rId21" xr:uid="{454C94D8-4DC6-49CD-A410-D42FAF10EB15}"/>
     <hyperlink ref="Z78" r:id="rId22" xr:uid="{995ED0EF-32F2-4DB4-B039-4E3822903D88}"/>
+    <hyperlink ref="Z79" r:id="rId23" xr:uid="{3BC7C50B-98E2-4EA6-AEEC-6A15B1E63BCB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
-  <drawing r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
+  <drawing r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>